<commit_message>
Updated spreadsheet for fall
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2017fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2017fall.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Box Sync\teaching\_phy132_2017\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="179" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -552,175 +552,189 @@
     <t>New by Matt 2015</t>
   </si>
   <si>
-    <t>1 Measuring and Graphing Horizontal Motion</t>
-  </si>
-  <si>
-    <t>2 Walking Speed</t>
-  </si>
-  <si>
-    <t>3 Converting Units</t>
-  </si>
-  <si>
-    <t>4 Measurement of Length, Mass, Volume, and Density</t>
-  </si>
-  <si>
-    <t>5 Determining Pi</t>
-  </si>
-  <si>
-    <t>6 Position vs. Time Graphs</t>
-  </si>
-  <si>
-    <t>7 Velocity vs. Time Graphs</t>
-  </si>
-  <si>
-    <t>8 Relating Position and Velocity Graphs</t>
-  </si>
-  <si>
-    <t>9 Instantaneous Velocity</t>
-  </si>
-  <si>
-    <t>10 Changing Motion</t>
-  </si>
-  <si>
-    <t>11 Slowing Down, Speeding Up, and Turning</t>
-  </si>
-  <si>
-    <t>12 Equations to Defi_x001C_ne Velocity and Acceleratio</t>
-  </si>
-  <si>
-    <t>13 Measurement and Uncertainty</t>
-  </si>
-  <si>
-    <t>14 Measurement, Uncertainty, and Variation</t>
-  </si>
-  <si>
-    <t>15 Gravity and Free Fall</t>
-  </si>
-  <si>
-    <t>16 Acceleration of Gravity</t>
-  </si>
-  <si>
-    <t>17 Human Reaction Time</t>
-  </si>
-  <si>
-    <t>18 The Tossed Ball</t>
-  </si>
-  <si>
-    <t>19 Independence of Vertical and Horizontal Motion</t>
-  </si>
-  <si>
-    <t>20 The Ski Jump</t>
-  </si>
-  <si>
-    <t>21 Projectile Motion</t>
-  </si>
-  <si>
-    <t>22 Vector Addition Exercises</t>
-  </si>
-  <si>
-    <t>23 Uniform Circular Motion</t>
-  </si>
-  <si>
-    <t>24 Force and Motion I</t>
-  </si>
-  <si>
-    <t>25 Force and Motion II</t>
-  </si>
-  <si>
-    <t>26 Combining Forces</t>
-  </si>
-  <si>
-    <t>27 Force, Mass and Acceleration</t>
-  </si>
-  <si>
-    <t>28 Newton's 3rd Law, Tension, and Normal Forces</t>
-  </si>
-  <si>
-    <t>29 Atwood's Machine</t>
-  </si>
-  <si>
-    <t>30 Friction and Applying the Laws of Motion</t>
-  </si>
-  <si>
-    <t>31 Check Your Units!</t>
-  </si>
-  <si>
-    <t>32 The Electrical and Gravitational Forces</t>
-  </si>
-  <si>
-    <t>33 Centripetal Force</t>
-  </si>
-  <si>
-    <t>34 Kepler's Laws</t>
-  </si>
-  <si>
-    <t>35 Work and Power</t>
-  </si>
-  <si>
-    <t>36 Work and Kinetic Energy</t>
-  </si>
-  <si>
-    <t>37 Conservation of Mechanical Energy</t>
-  </si>
-  <si>
-    <t>38 Weighing an Electron</t>
-  </si>
-  <si>
-    <t>39 Conservative and Non-Conservative Forces</t>
-  </si>
-  <si>
-    <t>40 Momentum and Momentum Change</t>
-  </si>
-  <si>
-    <t>41 Impulse, Momentum, and Interactions</t>
-  </si>
-  <si>
-    <t>42 Newton's Laws and Momentum Conservation</t>
-  </si>
-  <si>
-    <t>43 Momentum Conservation and Center of Mass</t>
-  </si>
-  <si>
-    <t>44 Two-Dimensional Collisions</t>
-  </si>
-  <si>
-    <t>45 Connecting Angular Displacement with Linear Displacement along the Arc</t>
-  </si>
-  <si>
-    <t>46 Introduction to Rotation</t>
-  </si>
-  <si>
-    <t>47 Newton's Second Law for Rotation</t>
-  </si>
-  <si>
-    <t>48 Rolling</t>
-  </si>
-  <si>
-    <t>49 Moment of Inertia</t>
-  </si>
-  <si>
-    <t>50 Angular Momentum and Torque as Vectors</t>
-  </si>
-  <si>
-    <t>51 Conservation of Angular Momentum</t>
-  </si>
-  <si>
-    <t>52 Hooke's Law</t>
-  </si>
-  <si>
-    <t>53 Periodic Motion</t>
-  </si>
-  <si>
-    <t>54 The Period of a Pendulum</t>
-  </si>
-  <si>
-    <t>55 Air Column Resonance</t>
-  </si>
-  <si>
-    <t>56 Galilean Relativity</t>
-  </si>
-  <si>
-    <t>57 The Twins Paradox</t>
+    <t>Measuring and Graphing Horizontal Motion</t>
+  </si>
+  <si>
+    <t>Walking Speed</t>
+  </si>
+  <si>
+    <t>Converting Units</t>
+  </si>
+  <si>
+    <t>Measurement of Length, Mass, Volume, and Density</t>
+  </si>
+  <si>
+    <t>Determining Pi</t>
+  </si>
+  <si>
+    <t>Position vs. Time Graphs</t>
+  </si>
+  <si>
+    <t>Velocity vs. Time Graphs</t>
+  </si>
+  <si>
+    <t>Relating Position and Velocity Graphs</t>
+  </si>
+  <si>
+    <t>Instantaneous Velocity</t>
+  </si>
+  <si>
+    <t>Slowing Down, Speeding Up, and Turning</t>
+  </si>
+  <si>
+    <t>Measurement and Uncertainty</t>
+  </si>
+  <si>
+    <t>Measurement, Uncertainty, and Variation</t>
+  </si>
+  <si>
+    <t>Gravity and Free Fall</t>
+  </si>
+  <si>
+    <t>Acceleration of Gravity</t>
+  </si>
+  <si>
+    <t>Human Reaction Time</t>
+  </si>
+  <si>
+    <t>The Tossed Ball</t>
+  </si>
+  <si>
+    <t>Independence of Vertical and Horizontal Motion</t>
+  </si>
+  <si>
+    <t>The Ski Jump</t>
+  </si>
+  <si>
+    <t>Projectile Motion</t>
+  </si>
+  <si>
+    <t>Vector Addition Exercises</t>
+  </si>
+  <si>
+    <t>Uniform Circular Motion</t>
+  </si>
+  <si>
+    <t>Force and Motion I</t>
+  </si>
+  <si>
+    <t>Force and Motion II</t>
+  </si>
+  <si>
+    <t>Combining Forces</t>
+  </si>
+  <si>
+    <t>Force, Mass and Acceleration</t>
+  </si>
+  <si>
+    <t>Newton's 3rd Law, Tension, and Normal Forces</t>
+  </si>
+  <si>
+    <t>Atwood's Machine</t>
+  </si>
+  <si>
+    <t>Friction and Applying the Laws of Motion</t>
+  </si>
+  <si>
+    <t>Check Your Units!</t>
+  </si>
+  <si>
+    <t>The Electrical and Gravitational Forces</t>
+  </si>
+  <si>
+    <t>Centripetal Force</t>
+  </si>
+  <si>
+    <t>Kepler's Laws</t>
+  </si>
+  <si>
+    <t>Work and Power</t>
+  </si>
+  <si>
+    <t>Work and Kinetic Energy</t>
+  </si>
+  <si>
+    <t>Conservation of Mechanical Energy</t>
+  </si>
+  <si>
+    <t>Weighing an Electron</t>
+  </si>
+  <si>
+    <t>Conservative and Non-Conservative Forces</t>
+  </si>
+  <si>
+    <t>Momentum and Momentum Change</t>
+  </si>
+  <si>
+    <t>Impulse, Momentum, and Interactions</t>
+  </si>
+  <si>
+    <t>Newton's Laws and Momentum Conservation</t>
+  </si>
+  <si>
+    <t>Momentum Conservation and Center of Mass</t>
+  </si>
+  <si>
+    <t>Two-Dimensional Collisions</t>
+  </si>
+  <si>
+    <t>Connecting Angular Displacement with Linear Displacement along the Arc</t>
+  </si>
+  <si>
+    <t>Introduction to Rotation</t>
+  </si>
+  <si>
+    <t>Newton's Second Law for Rotation</t>
+  </si>
+  <si>
+    <t>Rolling</t>
+  </si>
+  <si>
+    <t>Moment of Inertia</t>
+  </si>
+  <si>
+    <t>Angular Momentum and Torque as Vectors</t>
+  </si>
+  <si>
+    <t>Conservation of Angular Momentum</t>
+  </si>
+  <si>
+    <t>Hooke's Law</t>
+  </si>
+  <si>
+    <t>Periodic Motion</t>
+  </si>
+  <si>
+    <t>The Period of a Pendulum</t>
+  </si>
+  <si>
+    <t>Air Column Resonance</t>
+  </si>
+  <si>
+    <t>Galilean Relativity</t>
+  </si>
+  <si>
+    <t>The Twins Paradox</t>
+  </si>
+  <si>
+    <t>2017 Mariama</t>
+  </si>
+  <si>
+    <t>Equations to Define Velocity and Acceleration</t>
+  </si>
+  <si>
+    <t>Changing Motion</t>
+  </si>
+  <si>
+    <t>2016 fall
+Jack</t>
+  </si>
+  <si>
+    <t>2016 fall Christine</t>
+  </si>
+  <si>
+    <t>2017 
+Dr. Staff</t>
   </si>
 </sst>
 </file>
@@ -1352,7 +1366,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1548,8 +1562,14 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="44">
@@ -1598,7 +1618,91 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="15">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFCDFFCD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF99FF99"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1931,8 +2035,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P78" sqref="P78"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1941,10 +2045,12 @@
     <col min="2" max="2" width="44" style="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8.109375" style="14" customWidth="1"/>
     <col min="4" max="8" width="5.88671875" style="14" customWidth="1"/>
-    <col min="9" max="9" width="28.44140625" style="20" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="8.77734375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.77734375" style="20" customWidth="1"/>
-    <col min="13" max="15" width="8.77734375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="28.44140625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="10.109375" style="36" customWidth="1"/>
+    <col min="11" max="11" width="10.21875" style="36" customWidth="1"/>
+    <col min="12" max="13" width="8.77734375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.77734375" style="20" customWidth="1"/>
+    <col min="15" max="15" width="8.77734375" style="2" customWidth="1"/>
     <col min="16" max="16" width="11" style="3" customWidth="1"/>
     <col min="17" max="17" width="2.44140625" style="3" customWidth="1"/>
     <col min="18" max="18" width="10.33203125" style="3" customWidth="1"/>
@@ -1981,15 +2087,23 @@
         <v>90</v>
       </c>
       <c r="J1" s="49" t="s">
+        <v>180</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>181</v>
+      </c>
+      <c r="L1" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="K1" s="49" t="s">
+      <c r="M1" s="49" t="s">
         <v>114</v>
       </c>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
+      <c r="N1" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="O1" s="49" t="s">
+        <v>182</v>
+      </c>
       <c r="P1" s="52" t="s">
         <v>103</v>
       </c>
@@ -2021,18 +2135,20 @@
       <c r="G2" s="56"/>
       <c r="H2" s="56"/>
       <c r="I2" s="57"/>
-      <c r="J2" s="58">
-        <v>1</v>
-      </c>
-      <c r="K2" s="58">
-        <v>1</v>
-      </c>
-      <c r="L2" s="59"/>
-      <c r="M2" s="55"/>
-      <c r="N2" s="55"/>
+      <c r="J2" s="68">
+        <v>1</v>
+      </c>
+      <c r="K2" s="68"/>
+      <c r="L2" s="58">
+        <v>1</v>
+      </c>
+      <c r="M2" s="58">
+        <v>1</v>
+      </c>
+      <c r="N2" s="59"/>
       <c r="O2" s="55"/>
       <c r="P2" s="75">
-        <f>SUM(J2:O2)</f>
+        <f>SUM(L2:O2)</f>
         <v>2</v>
       </c>
       <c r="Q2" s="80"/>
@@ -2064,15 +2180,17 @@
       <c r="J3" s="63">
         <v>1</v>
       </c>
-      <c r="K3" s="63">
-        <v>1</v>
-      </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="60"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63">
+        <v>1</v>
+      </c>
+      <c r="M3" s="63">
+        <v>1</v>
+      </c>
       <c r="N3" s="60"/>
       <c r="O3" s="60"/>
       <c r="P3" s="76">
-        <f t="shared" ref="P3:P54" si="0">SUM(J3:O3)</f>
+        <f>SUM(L3:O3)</f>
         <v>2</v>
       </c>
       <c r="Q3" s="80"/>
@@ -2100,21 +2218,27 @@
         <v>1</v>
       </c>
       <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
+      <c r="G4" s="14">
+        <v>1</v>
+      </c>
+      <c r="H4" s="14">
+        <v>1</v>
+      </c>
       <c r="I4" s="22"/>
       <c r="J4" s="36">
         <v>1</v>
       </c>
-      <c r="K4" s="36">
+      <c r="K4" s="36"/>
+      <c r="L4" s="36">
+        <v>1</v>
+      </c>
+      <c r="M4" s="36">
         <v>0.5</v>
       </c>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
       <c r="N4" s="36"/>
       <c r="O4" s="36"/>
       <c r="P4" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L4:O4)</f>
         <v>1.5</v>
       </c>
       <c r="Q4" s="5"/>
@@ -2138,13 +2262,12 @@
         <v>2</v>
       </c>
       <c r="I5" s="22"/>
-      <c r="K5" s="2">
+      <c r="M5" s="2">
         <v>0.75</v>
       </c>
-      <c r="M5" s="34"/>
-      <c r="O5" s="85"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L5:O5)</f>
         <v>0.75</v>
       </c>
       <c r="Q5" s="5"/>
@@ -2166,16 +2289,14 @@
         <v>2</v>
       </c>
       <c r="I6" s="22"/>
-      <c r="J6" s="36"/>
-      <c r="K6" s="36">
-        <v>0</v>
-      </c>
       <c r="L6" s="36"/>
-      <c r="M6" s="36"/>
+      <c r="M6" s="36">
+        <v>0</v>
+      </c>
       <c r="N6" s="36"/>
-      <c r="O6" s="6"/>
+      <c r="O6" s="36"/>
       <c r="P6" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L6:O6)</f>
         <v>0</v>
       </c>
       <c r="Q6" s="5"/>
@@ -2202,16 +2323,16 @@
       <c r="G7" s="14"/>
       <c r="H7" s="14"/>
       <c r="I7" s="22"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="34">
-        <v>0</v>
-      </c>
-      <c r="L7" s="20"/>
-      <c r="M7" s="34"/>
-      <c r="N7" s="2"/>
+      <c r="J7" s="36"/>
+      <c r="K7" s="36"/>
+      <c r="L7" s="2"/>
+      <c r="M7" s="34">
+        <v>0</v>
+      </c>
+      <c r="N7" s="20"/>
       <c r="O7" s="34"/>
       <c r="P7" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L7:O7)</f>
         <v>0</v>
       </c>
       <c r="Q7" s="5"/>
@@ -2228,13 +2349,12 @@
         <v>2</v>
       </c>
       <c r="I8" s="22"/>
-      <c r="K8" s="2">
-        <v>0</v>
-      </c>
-      <c r="M8" s="34"/>
-      <c r="O8" s="33"/>
+      <c r="M8" s="2">
+        <v>0</v>
+      </c>
+      <c r="O8" s="34"/>
       <c r="P8" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L8:O8)</f>
         <v>0</v>
       </c>
       <c r="Q8" s="5"/>
@@ -2257,17 +2377,28 @@
       <c r="E9" s="14">
         <v>3</v>
       </c>
+      <c r="G9" s="14">
+        <v>2</v>
+      </c>
+      <c r="H9" s="14">
+        <v>2</v>
+      </c>
       <c r="I9" s="22"/>
-      <c r="J9" s="2">
-        <v>1</v>
-      </c>
-      <c r="K9" s="2">
-        <v>1</v>
-      </c>
-      <c r="M9" s="34"/>
+      <c r="J9" s="36">
+        <v>1</v>
+      </c>
+      <c r="K9" s="36">
+        <v>1</v>
+      </c>
+      <c r="L9" s="2">
+        <v>1</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1</v>
+      </c>
       <c r="O9" s="34"/>
       <c r="P9" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L9:O9)</f>
         <v>2</v>
       </c>
       <c r="Q9" s="5"/>
@@ -2290,19 +2421,29 @@
       <c r="E10" s="14">
         <v>4</v>
       </c>
+      <c r="G10" s="14">
+        <v>3</v>
+      </c>
+      <c r="H10" s="14">
+        <v>3</v>
+      </c>
       <c r="I10" s="22"/>
-      <c r="J10" s="34">
-        <v>1</v>
-      </c>
-      <c r="K10" s="34">
-        <v>1</v>
-      </c>
-      <c r="L10" s="36"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
+      <c r="J10" s="36">
+        <v>1</v>
+      </c>
+      <c r="K10" s="36">
+        <v>1</v>
+      </c>
+      <c r="L10" s="34">
+        <v>1</v>
+      </c>
+      <c r="M10" s="34">
+        <v>1</v>
+      </c>
+      <c r="N10" s="36"/>
       <c r="O10" s="34"/>
       <c r="P10" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L10:O10)</f>
         <v>2</v>
       </c>
       <c r="Q10" s="5"/>
@@ -2325,19 +2466,26 @@
       <c r="E11" s="14">
         <v>5</v>
       </c>
+      <c r="G11" s="14">
+        <v>4</v>
+      </c>
+      <c r="H11" s="14">
+        <v>4</v>
+      </c>
       <c r="I11" s="22"/>
-      <c r="J11" s="34">
-        <v>1</v>
-      </c>
-      <c r="K11" s="34">
+      <c r="K11" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L11" s="34">
+        <v>1</v>
+      </c>
+      <c r="M11" s="34">
         <v>0.75</v>
       </c>
-      <c r="L11" s="36"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
+      <c r="N11" s="36"/>
       <c r="O11" s="34"/>
       <c r="P11" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L11:O11)</f>
         <v>1.75</v>
       </c>
       <c r="Q11" s="5"/>
@@ -2360,16 +2508,17 @@
         <v>3</v>
       </c>
       <c r="I12" s="22"/>
-      <c r="J12" s="34"/>
-      <c r="K12" s="34">
-        <v>0</v>
-      </c>
-      <c r="L12" s="36"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
+      <c r="K12" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34">
+        <v>0</v>
+      </c>
+      <c r="N12" s="36"/>
       <c r="O12" s="34"/>
       <c r="P12" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L12:O12)</f>
         <v>0</v>
       </c>
       <c r="Q12" s="15"/>
@@ -2386,7 +2535,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>131</v>
+        <v>179</v>
       </c>
       <c r="C13" s="14">
         <v>12</v>
@@ -2394,19 +2543,26 @@
       <c r="E13" s="14">
         <v>6</v>
       </c>
+      <c r="G13" s="14">
+        <v>5</v>
+      </c>
+      <c r="H13" s="14">
+        <v>5</v>
+      </c>
       <c r="I13" s="22"/>
-      <c r="J13" s="34">
-        <v>1</v>
-      </c>
-      <c r="K13" s="34">
-        <v>1</v>
-      </c>
-      <c r="L13" s="36"/>
-      <c r="M13" s="34"/>
-      <c r="N13" s="34"/>
+      <c r="J13" s="36">
+        <v>1</v>
+      </c>
+      <c r="L13" s="34">
+        <v>1</v>
+      </c>
+      <c r="M13" s="34">
+        <v>1</v>
+      </c>
+      <c r="N13" s="36"/>
       <c r="O13" s="34"/>
       <c r="P13" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L13:O13)</f>
         <v>2</v>
       </c>
       <c r="Q13" s="5"/>
@@ -2421,7 +2577,7 @@
     </row>
     <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C14" s="14">
         <v>13</v>
@@ -2429,19 +2585,26 @@
       <c r="E14" s="14">
         <v>7</v>
       </c>
+      <c r="G14" s="14">
+        <v>6</v>
+      </c>
+      <c r="H14" s="14">
+        <v>6</v>
+      </c>
       <c r="I14" s="22"/>
-      <c r="J14" s="34">
-        <v>1</v>
-      </c>
-      <c r="K14" s="34">
+      <c r="K14" s="36">
+        <v>1</v>
+      </c>
+      <c r="L14" s="34">
+        <v>1</v>
+      </c>
+      <c r="M14" s="34">
         <v>0.5</v>
       </c>
-      <c r="L14" s="36"/>
-      <c r="M14" s="34"/>
-      <c r="N14" s="34"/>
+      <c r="N14" s="36"/>
       <c r="O14" s="34"/>
       <c r="P14" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L14:O14)</f>
         <v>1.5</v>
       </c>
       <c r="Q14" s="5"/>
@@ -2457,7 +2620,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>133</v>
+        <v>178</v>
       </c>
       <c r="C15" s="14">
         <v>6</v>
@@ -2466,16 +2629,14 @@
         <v>8</v>
       </c>
       <c r="I15" s="22"/>
-      <c r="J15" s="34"/>
-      <c r="K15" s="34">
-        <v>0</v>
-      </c>
-      <c r="L15" s="36"/>
-      <c r="M15" s="34"/>
-      <c r="N15" s="34"/>
+      <c r="L15" s="34"/>
+      <c r="M15" s="34">
+        <v>0</v>
+      </c>
+      <c r="N15" s="36"/>
       <c r="O15" s="34"/>
       <c r="P15" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L15:O15)</f>
         <v>0</v>
       </c>
       <c r="Q15" s="5"/>
@@ -2494,22 +2655,23 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C16" s="14">
         <v>3</v>
       </c>
       <c r="I16" s="22"/>
-      <c r="J16" s="34"/>
-      <c r="K16" s="34">
-        <v>0</v>
-      </c>
-      <c r="L16" s="36"/>
-      <c r="M16" s="34"/>
-      <c r="N16" s="34"/>
+      <c r="K16" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="L16" s="34"/>
+      <c r="M16" s="34">
+        <v>0</v>
+      </c>
+      <c r="N16" s="36"/>
       <c r="O16" s="34"/>
       <c r="P16" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L16:O16)</f>
         <v>0</v>
       </c>
       <c r="Q16" s="5"/>
@@ -2528,7 +2690,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C17" s="14">
         <v>5</v>
@@ -2537,18 +2699,16 @@
         <v>9</v>
       </c>
       <c r="I17" s="22"/>
-      <c r="J17" s="34">
+      <c r="L17" s="34">
         <v>0.5</v>
       </c>
-      <c r="K17" s="34">
+      <c r="M17" s="34">
         <v>0.75</v>
       </c>
-      <c r="L17" s="36"/>
-      <c r="M17" s="34"/>
-      <c r="N17" s="34"/>
+      <c r="N17" s="36"/>
       <c r="O17" s="34"/>
       <c r="P17" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L17:O17)</f>
         <v>1.25</v>
       </c>
       <c r="Q17" s="5"/>
@@ -2567,7 +2727,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C18" s="14">
         <v>3</v>
@@ -2575,19 +2735,29 @@
       <c r="E18" s="14">
         <v>10</v>
       </c>
+      <c r="G18" s="14">
+        <v>7</v>
+      </c>
+      <c r="H18" s="14">
+        <v>7</v>
+      </c>
       <c r="I18" s="22"/>
-      <c r="J18" s="34">
-        <v>1</v>
-      </c>
-      <c r="K18" s="34">
+      <c r="J18" s="36">
+        <v>1</v>
+      </c>
+      <c r="K18" s="36">
+        <v>1</v>
+      </c>
+      <c r="L18" s="34">
+        <v>1</v>
+      </c>
+      <c r="M18" s="34">
         <v>0.75</v>
       </c>
-      <c r="L18" s="36"/>
-      <c r="M18" s="34"/>
-      <c r="N18" s="34"/>
+      <c r="N18" s="36"/>
       <c r="O18" s="34"/>
       <c r="P18" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L18:O18)</f>
         <v>1.75</v>
       </c>
       <c r="Q18" s="5"/>
@@ -2606,22 +2776,20 @@
     </row>
     <row r="19" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C19" s="14">
         <v>2</v>
       </c>
       <c r="I19" s="22"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34">
-        <v>0</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="34"/>
-      <c r="N19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34">
+        <v>0</v>
+      </c>
+      <c r="N19" s="36"/>
       <c r="O19" s="34"/>
       <c r="P19" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L19:O19)</f>
         <v>0</v>
       </c>
       <c r="Q19" s="15"/>
@@ -2640,22 +2808,20 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
       </c>
       <c r="I20" s="22"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34">
-        <v>0</v>
-      </c>
-      <c r="L20" s="36"/>
-      <c r="M20" s="34"/>
-      <c r="N20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34">
+        <v>0</v>
+      </c>
+      <c r="N20" s="36"/>
       <c r="O20" s="34"/>
       <c r="P20" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L20:O20)</f>
         <v>0</v>
       </c>
       <c r="Q20" s="15"/>
@@ -2667,22 +2833,20 @@
     </row>
     <row r="21" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C21" s="14">
         <v>2</v>
       </c>
       <c r="I21" s="22"/>
-      <c r="J21" s="34"/>
-      <c r="K21" s="34">
-        <v>0</v>
-      </c>
-      <c r="L21" s="36"/>
-      <c r="M21" s="34"/>
-      <c r="N21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34">
+        <v>0</v>
+      </c>
+      <c r="N21" s="36"/>
       <c r="O21" s="34"/>
       <c r="P21" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L21:O21)</f>
         <v>0</v>
       </c>
       <c r="Q21" s="15"/>
@@ -2697,19 +2861,21 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C22" s="14">
         <v>1</v>
       </c>
       <c r="I22" s="22"/>
-      <c r="K22" s="2">
-        <v>0</v>
-      </c>
-      <c r="M22" s="34"/>
+      <c r="K22" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="M22" s="2">
+        <v>0</v>
+      </c>
       <c r="O22" s="34"/>
       <c r="P22" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L22:O22)</f>
         <v>0</v>
       </c>
       <c r="Q22" s="15"/>
@@ -2732,19 +2898,18 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C23" s="14">
         <v>2</v>
       </c>
       <c r="I23" s="22"/>
-      <c r="K23" s="2">
-        <v>0</v>
-      </c>
-      <c r="M23" s="34"/>
+      <c r="M23" s="2">
+        <v>0</v>
+      </c>
       <c r="O23" s="34"/>
       <c r="P23" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L23:O23)</f>
         <v>0</v>
       </c>
       <c r="Q23" s="15"/>
@@ -2760,7 +2925,7 @@
         <v>7</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" ref="U23:U31" si="1">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
+        <f t="shared" ref="U23:U31" si="0">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
         <v>25.870000000000005</v>
       </c>
       <c r="V23" s="33"/>
@@ -2771,7 +2936,7 @@
     <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C24" s="14">
         <v>3</v>
@@ -2781,21 +2946,29 @@
         <v>11</v>
       </c>
       <c r="F24" s="14"/>
-      <c r="G24" s="14"/>
-      <c r="H24" s="14"/>
+      <c r="G24" s="14">
+        <v>8</v>
+      </c>
+      <c r="H24" s="14">
+        <v>8</v>
+      </c>
       <c r="I24" s="22"/>
-      <c r="J24" s="2">
-        <v>1</v>
-      </c>
-      <c r="K24" s="2">
-        <v>1</v>
-      </c>
-      <c r="L24" s="20"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="2"/>
+      <c r="J24" s="36">
+        <v>1</v>
+      </c>
+      <c r="K24" s="36">
+        <v>1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>1</v>
+      </c>
+      <c r="M24" s="2">
+        <v>1</v>
+      </c>
+      <c r="N24" s="20"/>
       <c r="O24" s="34"/>
       <c r="P24" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L24:O24)</f>
         <v>2</v>
       </c>
       <c r="Q24" s="15"/>
@@ -2811,7 +2984,7 @@
         <v>7</v>
       </c>
       <c r="U24" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>22.490000000000002</v>
       </c>
       <c r="V24" s="33"/>
@@ -2821,7 +2994,7 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C25" s="14">
         <v>4</v>
@@ -2829,16 +3002,15 @@
       <c r="I25" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="J25" s="2">
-        <v>1</v>
-      </c>
-      <c r="K25" s="2">
-        <v>0</v>
-      </c>
-      <c r="M25" s="34"/>
+      <c r="L25" s="2">
+        <v>1</v>
+      </c>
+      <c r="M25" s="2">
+        <v>0</v>
+      </c>
       <c r="O25" s="34"/>
       <c r="P25" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L25:O25)</f>
         <v>1</v>
       </c>
       <c r="Q25" s="15"/>
@@ -2854,7 +3026,7 @@
         <v>7</v>
       </c>
       <c r="U25" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>20.605</v>
       </c>
       <c r="V25" s="33"/>
@@ -2864,7 +3036,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C26" s="14">
         <v>6</v>
@@ -2872,17 +3044,25 @@
       <c r="E26" s="14">
         <v>12</v>
       </c>
+      <c r="G26" s="14">
+        <v>9</v>
+      </c>
+      <c r="H26" s="14">
+        <v>9</v>
+      </c>
       <c r="I26" s="22"/>
-      <c r="J26" s="2">
-        <v>1</v>
-      </c>
-      <c r="K26" s="2">
-        <v>1</v>
-      </c>
-      <c r="M26" s="34"/>
+      <c r="K26" s="36">
+        <v>1</v>
+      </c>
+      <c r="L26" s="2">
+        <v>1</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
       <c r="O26" s="34"/>
       <c r="P26" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L26:O26)</f>
         <v>2</v>
       </c>
       <c r="Q26" s="15"/>
@@ -2898,7 +3078,7 @@
         <v>6</v>
       </c>
       <c r="U26" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>18.134999999999998</v>
       </c>
       <c r="V26" s="33"/>
@@ -2911,7 +3091,7 @@
         <v>120</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C27" s="13">
         <v>12</v>
@@ -2921,21 +3101,29 @@
         <v>13</v>
       </c>
       <c r="F27" s="13"/>
-      <c r="G27" s="13"/>
-      <c r="H27" s="13"/>
+      <c r="G27" s="13">
+        <v>10</v>
+      </c>
+      <c r="H27" s="13">
+        <v>10</v>
+      </c>
       <c r="I27" s="21"/>
-      <c r="J27" s="12">
-        <v>1</v>
-      </c>
-      <c r="K27" s="12">
-        <v>1</v>
-      </c>
-      <c r="L27" s="12"/>
-      <c r="M27" s="35"/>
+      <c r="J27" s="35">
+        <v>1</v>
+      </c>
+      <c r="K27" s="35">
+        <v>0.5</v>
+      </c>
+      <c r="L27" s="12">
+        <v>1</v>
+      </c>
+      <c r="M27" s="12">
+        <v>1</v>
+      </c>
       <c r="N27" s="12"/>
       <c r="O27" s="35"/>
       <c r="P27" s="78">
-        <f t="shared" si="0"/>
+        <f>SUM(L27:O27)</f>
         <v>2</v>
       </c>
       <c r="Q27" s="15"/>
@@ -2951,13 +3139,13 @@
         <v>6</v>
       </c>
       <c r="U27" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>13.065000000000001</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C28" s="14">
         <v>8</v>
@@ -2965,17 +3153,22 @@
       <c r="E28" s="14">
         <v>14</v>
       </c>
+      <c r="G28" s="14">
+        <v>11</v>
+      </c>
+      <c r="H28" s="14">
+        <v>11</v>
+      </c>
       <c r="I28" s="22"/>
-      <c r="J28" s="2">
-        <v>1</v>
-      </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
+        <v>1</v>
+      </c>
+      <c r="M28" s="2">
         <v>0.8</v>
       </c>
-      <c r="M28" s="34"/>
       <c r="O28" s="34"/>
       <c r="P28" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L28:O28)</f>
         <v>1.8</v>
       </c>
       <c r="Q28" s="15"/>
@@ -2991,13 +3184,13 @@
         <v>0</v>
       </c>
       <c r="U28" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C29" s="14">
         <v>7</v>
@@ -3006,13 +3199,12 @@
         <v>15</v>
       </c>
       <c r="I29" s="22"/>
-      <c r="K29" s="2">
+      <c r="M29" s="2">
         <v>0.7</v>
       </c>
-      <c r="M29" s="34"/>
       <c r="O29" s="34"/>
       <c r="P29" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L29:O29)</f>
         <v>0.7</v>
       </c>
       <c r="Q29" s="15"/>
@@ -3028,13 +3220,13 @@
         <v>0</v>
       </c>
       <c r="U29" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C30" s="14">
         <v>9</v>
@@ -3042,17 +3234,24 @@
       <c r="E30" s="14">
         <v>16</v>
       </c>
+      <c r="G30" s="14">
+        <v>12</v>
+      </c>
+      <c r="H30" s="14">
+        <v>12</v>
+      </c>
       <c r="I30" s="22"/>
-      <c r="J30" s="34"/>
-      <c r="K30" s="34">
+      <c r="K30" s="36">
+        <v>1</v>
+      </c>
+      <c r="L30" s="34"/>
+      <c r="M30" s="34">
         <v>0.5</v>
       </c>
-      <c r="L30" s="36"/>
-      <c r="M30" s="34"/>
-      <c r="N30" s="34"/>
+      <c r="N30" s="36"/>
       <c r="O30" s="34"/>
       <c r="P30" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L30:O30)</f>
         <v>0.5</v>
       </c>
       <c r="Q30" s="15"/>
@@ -3068,13 +3267,13 @@
         <v>0</v>
       </c>
       <c r="U30" s="8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C31" s="14">
         <v>7</v>
@@ -3082,19 +3281,29 @@
       <c r="E31" s="14">
         <v>17</v>
       </c>
+      <c r="G31" s="14">
+        <v>13</v>
+      </c>
+      <c r="H31" s="14">
+        <v>13</v>
+      </c>
       <c r="I31" s="22"/>
-      <c r="J31" s="34">
-        <v>1</v>
-      </c>
-      <c r="K31" s="34">
+      <c r="J31" s="36">
+        <v>1</v>
+      </c>
+      <c r="K31" s="36">
+        <v>1</v>
+      </c>
+      <c r="L31" s="34">
+        <v>1</v>
+      </c>
+      <c r="M31" s="34">
         <v>0.5</v>
       </c>
-      <c r="L31" s="36"/>
-      <c r="M31" s="34"/>
-      <c r="N31" s="34"/>
+      <c r="N31" s="36"/>
       <c r="O31" s="34"/>
       <c r="P31" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L31:O31)</f>
         <v>1.5</v>
       </c>
       <c r="Q31" s="15"/>
@@ -3110,14 +3319,14 @@
         <v>0</v>
       </c>
       <c r="U31" s="9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>3.9000000000000004</v>
       </c>
     </row>
     <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="23" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C32" s="14">
         <v>4</v>
@@ -3128,16 +3337,16 @@
       <c r="G32" s="14"/>
       <c r="H32" s="14"/>
       <c r="I32" s="22"/>
-      <c r="J32" s="34"/>
-      <c r="K32" s="34">
-        <v>1</v>
-      </c>
-      <c r="L32" s="36"/>
-      <c r="M32" s="34"/>
-      <c r="N32" s="34"/>
+      <c r="J32" s="36"/>
+      <c r="K32" s="36"/>
+      <c r="L32" s="34"/>
+      <c r="M32" s="34">
+        <v>1</v>
+      </c>
+      <c r="N32" s="36"/>
       <c r="O32" s="34"/>
       <c r="P32" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L32:O32)</f>
         <v>1</v>
       </c>
       <c r="Q32" s="15"/>
@@ -3147,7 +3356,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C33" s="14">
         <v>5</v>
@@ -3155,26 +3364,36 @@
       <c r="E33" s="14">
         <v>18</v>
       </c>
+      <c r="G33" s="14">
+        <v>14</v>
+      </c>
+      <c r="H33" s="14">
+        <v>14</v>
+      </c>
       <c r="I33" s="22"/>
-      <c r="J33" s="34">
-        <v>1</v>
-      </c>
-      <c r="K33" s="34">
+      <c r="J33" s="36">
+        <v>1</v>
+      </c>
+      <c r="K33" s="36">
+        <v>1</v>
+      </c>
+      <c r="L33" s="34">
+        <v>1</v>
+      </c>
+      <c r="M33" s="34">
         <v>0.5</v>
       </c>
-      <c r="L33" s="36"/>
-      <c r="M33" s="34"/>
-      <c r="N33" s="34"/>
+      <c r="N33" s="36"/>
       <c r="O33" s="34"/>
       <c r="P33" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L33:O33)</f>
         <v>1.5</v>
       </c>
       <c r="Q33" s="15"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C34" s="14">
         <v>2</v>
@@ -3182,23 +3401,24 @@
       <c r="I34" s="22" t="s">
         <v>121</v>
       </c>
-      <c r="J34" s="34"/>
-      <c r="K34" s="34">
+      <c r="J34" s="36">
         <v>0.5</v>
       </c>
-      <c r="L34" s="36"/>
-      <c r="M34" s="34"/>
-      <c r="N34" s="34"/>
+      <c r="L34" s="34"/>
+      <c r="M34" s="34">
+        <v>0.5</v>
+      </c>
+      <c r="N34" s="36"/>
       <c r="O34" s="34"/>
       <c r="P34" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L34:O34)</f>
         <v>0.5</v>
       </c>
       <c r="Q34" s="15"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C35" s="14">
         <v>5</v>
@@ -3206,19 +3426,26 @@
       <c r="E35" s="14">
         <v>19</v>
       </c>
+      <c r="G35" s="14">
+        <v>15</v>
+      </c>
+      <c r="H35" s="14">
+        <v>15</v>
+      </c>
       <c r="I35" s="22"/>
-      <c r="J35" s="34">
-        <v>1</v>
-      </c>
-      <c r="K35" s="34">
-        <v>1</v>
-      </c>
-      <c r="L35" s="36"/>
-      <c r="M35" s="34"/>
-      <c r="N35" s="34"/>
+      <c r="K35" s="36">
+        <v>1</v>
+      </c>
+      <c r="L35" s="34">
+        <v>1</v>
+      </c>
+      <c r="M35" s="34">
+        <v>1</v>
+      </c>
+      <c r="N35" s="36"/>
       <c r="O35" s="34"/>
       <c r="P35" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L35:O35)</f>
         <v>2</v>
       </c>
       <c r="Q35" s="15"/>
@@ -3226,7 +3453,7 @@
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="C36" s="14">
         <v>8</v>
@@ -3234,19 +3461,23 @@
       <c r="E36" s="14">
         <v>20</v>
       </c>
+      <c r="G36" s="14">
+        <v>16</v>
+      </c>
+      <c r="H36" s="14">
+        <v>16</v>
+      </c>
       <c r="I36" s="22"/>
-      <c r="J36" s="34">
-        <v>1</v>
-      </c>
-      <c r="K36" s="34">
+      <c r="L36" s="34">
+        <v>1</v>
+      </c>
+      <c r="M36" s="34">
         <v>0.5</v>
       </c>
-      <c r="L36" s="36"/>
-      <c r="M36" s="34"/>
-      <c r="N36" s="34"/>
+      <c r="N36" s="36"/>
       <c r="O36" s="34"/>
       <c r="P36" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L36:O36)</f>
         <v>1.5</v>
       </c>
       <c r="Q36" s="15"/>
@@ -3254,19 +3485,30 @@
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C37" s="14">
         <v>4</v>
       </c>
+      <c r="G37" s="14">
+        <v>17</v>
+      </c>
+      <c r="H37" s="14">
+        <v>17</v>
+      </c>
       <c r="I37" s="22"/>
-      <c r="K37" s="2">
+      <c r="J37" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="K37" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="M37" s="2">
         <v>0.8</v>
       </c>
-      <c r="M37" s="34"/>
       <c r="O37" s="34"/>
       <c r="P37" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L37:O37)</f>
         <v>0.8</v>
       </c>
       <c r="Q37" s="15"/>
@@ -3278,7 +3520,7 @@
         <v>119</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C38" s="13">
         <v>6</v>
@@ -3288,21 +3530,29 @@
         <v>21</v>
       </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="13"/>
-      <c r="H38" s="13"/>
+      <c r="G38" s="13">
+        <v>18</v>
+      </c>
+      <c r="H38" s="13">
+        <v>18</v>
+      </c>
       <c r="I38" s="21"/>
-      <c r="J38" s="12">
-        <v>1</v>
-      </c>
-      <c r="K38" s="12">
-        <v>1</v>
-      </c>
-      <c r="L38" s="12"/>
-      <c r="M38" s="35"/>
+      <c r="J38" s="35">
+        <v>1</v>
+      </c>
+      <c r="K38" s="35">
+        <v>1</v>
+      </c>
+      <c r="L38" s="12">
+        <v>1</v>
+      </c>
+      <c r="M38" s="12">
+        <v>1</v>
+      </c>
       <c r="N38" s="12"/>
       <c r="O38" s="35"/>
       <c r="P38" s="78">
-        <f t="shared" si="0"/>
+        <f>SUM(L38:O38)</f>
         <v>2</v>
       </c>
       <c r="Q38" s="15"/>
@@ -3310,7 +3560,7 @@
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39" s="31" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C39" s="14">
         <v>6</v>
@@ -3318,19 +3568,26 @@
       <c r="E39" s="14">
         <v>22</v>
       </c>
+      <c r="G39" s="14">
+        <v>19</v>
+      </c>
+      <c r="H39" s="14">
+        <v>19</v>
+      </c>
       <c r="I39" s="22"/>
       <c r="J39" s="36">
         <v>1</v>
       </c>
-      <c r="K39" s="36">
+      <c r="L39" s="36">
+        <v>1</v>
+      </c>
+      <c r="M39" s="36">
         <v>0.75</v>
       </c>
-      <c r="L39" s="36"/>
-      <c r="M39" s="36"/>
       <c r="N39" s="36"/>
       <c r="O39" s="36"/>
       <c r="P39" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L39:O39)</f>
         <v>1.75</v>
       </c>
       <c r="Q39" s="15"/>
@@ -3340,7 +3597,7 @@
     <row r="40" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="31" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C40" s="14">
         <v>3</v>
@@ -3350,8 +3607,12 @@
         <v>23</v>
       </c>
       <c r="F40" s="14"/>
-      <c r="G40" s="14"/>
-      <c r="H40" s="14"/>
+      <c r="G40" s="14">
+        <v>20</v>
+      </c>
+      <c r="H40" s="14">
+        <v>20</v>
+      </c>
       <c r="I40" s="22"/>
       <c r="J40" s="36">
         <v>1</v>
@@ -3359,12 +3620,16 @@
       <c r="K40" s="36">
         <v>0.5</v>
       </c>
-      <c r="L40" s="36"/>
-      <c r="M40" s="36"/>
+      <c r="L40" s="36">
+        <v>1</v>
+      </c>
+      <c r="M40" s="36">
+        <v>0.5</v>
+      </c>
       <c r="N40" s="36"/>
       <c r="O40" s="36"/>
       <c r="P40" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L40:O40)</f>
         <v>1.5</v>
       </c>
       <c r="Q40" s="15"/>
@@ -3379,7 +3644,7 @@
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C41" s="14">
         <v>6</v>
@@ -3388,16 +3653,14 @@
         <v>24</v>
       </c>
       <c r="I41" s="22"/>
-      <c r="J41" s="36"/>
-      <c r="K41" s="36">
-        <v>1</v>
-      </c>
       <c r="L41" s="36"/>
-      <c r="M41" s="36"/>
+      <c r="M41" s="36">
+        <v>1</v>
+      </c>
       <c r="N41" s="36"/>
       <c r="O41" s="36"/>
       <c r="P41" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L41:O41)</f>
         <v>1</v>
       </c>
       <c r="Q41" s="15"/>
@@ -3409,7 +3672,7 @@
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C42" s="14">
         <v>5</v>
@@ -3417,19 +3680,29 @@
       <c r="E42" s="14">
         <v>25</v>
       </c>
+      <c r="G42" s="14">
+        <v>21</v>
+      </c>
+      <c r="H42" s="14">
+        <v>21</v>
+      </c>
       <c r="I42" s="22"/>
       <c r="J42" s="36">
         <v>1</v>
       </c>
       <c r="K42" s="36">
-        <v>0</v>
-      </c>
-      <c r="L42" s="36"/>
-      <c r="M42" s="36"/>
+        <v>1</v>
+      </c>
+      <c r="L42" s="36">
+        <v>1</v>
+      </c>
+      <c r="M42" s="36">
+        <v>0</v>
+      </c>
       <c r="N42" s="36"/>
       <c r="O42" s="36"/>
       <c r="P42" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L42:O42)</f>
         <v>1</v>
       </c>
       <c r="Q42" s="15"/>
@@ -3438,7 +3711,7 @@
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C43" s="14">
         <v>6</v>
@@ -3446,19 +3719,26 @@
       <c r="E43" s="14">
         <v>26</v>
       </c>
+      <c r="G43" s="14">
+        <v>22</v>
+      </c>
+      <c r="H43" s="14">
+        <v>22</v>
+      </c>
       <c r="I43" s="22"/>
-      <c r="J43" s="36">
-        <v>1</v>
-      </c>
       <c r="K43" s="36">
         <v>1</v>
       </c>
-      <c r="L43" s="36"/>
-      <c r="M43" s="36"/>
+      <c r="L43" s="36">
+        <v>1</v>
+      </c>
+      <c r="M43" s="36">
+        <v>1</v>
+      </c>
       <c r="N43" s="36"/>
       <c r="O43" s="36"/>
       <c r="P43" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L43:O43)</f>
         <v>2</v>
       </c>
       <c r="Q43" s="15"/>
@@ -3468,7 +3748,7 @@
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C44" s="14">
         <v>4</v>
@@ -3476,19 +3756,26 @@
       <c r="E44" s="14">
         <v>27</v>
       </c>
+      <c r="G44" s="14">
+        <v>23</v>
+      </c>
+      <c r="H44" s="14">
+        <v>23</v>
+      </c>
       <c r="I44" s="22"/>
-      <c r="J44" s="36">
-        <v>1</v>
-      </c>
       <c r="K44" s="36">
+        <v>1</v>
+      </c>
+      <c r="L44" s="36">
+        <v>1</v>
+      </c>
+      <c r="M44" s="36">
         <v>0.75</v>
       </c>
-      <c r="L44" s="36"/>
-      <c r="M44" s="36"/>
       <c r="N44" s="36"/>
       <c r="O44" s="36"/>
       <c r="P44" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L44:O44)</f>
         <v>1.75</v>
       </c>
       <c r="Q44" s="15"/>
@@ -3497,7 +3784,7 @@
     <row r="45" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C45" s="14">
         <v>7</v>
@@ -3507,8 +3794,12 @@
         <v>28</v>
       </c>
       <c r="F45" s="14"/>
-      <c r="G45" s="14"/>
-      <c r="H45" s="14"/>
+      <c r="G45" s="14">
+        <v>24</v>
+      </c>
+      <c r="H45" s="14">
+        <v>24</v>
+      </c>
       <c r="I45" s="22"/>
       <c r="J45" s="36">
         <v>1</v>
@@ -3516,12 +3807,16 @@
       <c r="K45" s="36">
         <v>1</v>
       </c>
-      <c r="L45" s="36"/>
-      <c r="M45" s="36"/>
+      <c r="L45" s="36">
+        <v>1</v>
+      </c>
+      <c r="M45" s="36">
+        <v>1</v>
+      </c>
       <c r="N45" s="36"/>
       <c r="O45" s="36"/>
       <c r="P45" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L45:O45)</f>
         <v>2</v>
       </c>
       <c r="Q45" s="15"/>
@@ -3537,7 +3832,7 @@
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C46" s="14">
         <v>6</v>
@@ -3545,24 +3840,34 @@
       <c r="E46" s="14">
         <v>29</v>
       </c>
+      <c r="G46" s="14">
+        <v>25</v>
+      </c>
+      <c r="H46" s="14">
+        <v>25</v>
+      </c>
       <c r="I46" s="22"/>
-      <c r="J46" s="36"/>
+      <c r="J46" s="36">
+        <v>1</v>
+      </c>
       <c r="K46" s="36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L46" s="36"/>
-      <c r="M46" s="36"/>
+      <c r="M46" s="36">
+        <v>0</v>
+      </c>
       <c r="N46" s="36"/>
       <c r="O46" s="36"/>
       <c r="P46" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L46:O46)</f>
         <v>0</v>
       </c>
       <c r="Q46" s="15"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C47" s="14">
         <v>5</v>
@@ -3570,17 +3875,28 @@
       <c r="E47" s="14">
         <v>30</v>
       </c>
+      <c r="G47" s="14">
+        <v>26</v>
+      </c>
+      <c r="H47" s="14">
+        <v>26</v>
+      </c>
       <c r="I47" s="22"/>
-      <c r="J47" s="2">
+      <c r="J47" s="36">
+        <v>1</v>
+      </c>
+      <c r="K47" s="36">
         <v>0.5</v>
       </c>
-      <c r="K47" s="2">
-        <v>1</v>
-      </c>
-      <c r="M47" s="34"/>
+      <c r="L47" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="M47" s="2">
+        <v>1</v>
+      </c>
       <c r="O47" s="34"/>
       <c r="P47" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L47:O47)</f>
         <v>1.5</v>
       </c>
       <c r="Q47" s="15"/>
@@ -3590,7 +3906,7 @@
         <v>118</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C48" s="13">
         <v>2</v>
@@ -3600,19 +3916,27 @@
         <v>31</v>
       </c>
       <c r="F48" s="13"/>
-      <c r="G48" s="13"/>
-      <c r="H48" s="13"/>
+      <c r="G48" s="13">
+        <v>27</v>
+      </c>
+      <c r="H48" s="13">
+        <v>27</v>
+      </c>
       <c r="I48" s="21"/>
-      <c r="J48" s="12"/>
-      <c r="K48" s="12">
-        <v>0</v>
+      <c r="J48" s="35">
+        <v>1</v>
+      </c>
+      <c r="K48" s="35">
+        <v>0.5</v>
       </c>
       <c r="L48" s="12"/>
-      <c r="M48" s="35"/>
+      <c r="M48" s="12">
+        <v>0</v>
+      </c>
       <c r="N48" s="12"/>
       <c r="O48" s="35"/>
       <c r="P48" s="78">
-        <f t="shared" si="0"/>
+        <f>SUM(L48:O48)</f>
         <v>0</v>
       </c>
       <c r="Q48" s="15"/>
@@ -3625,7 +3949,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C49" s="14">
         <v>7</v>
@@ -3633,17 +3957,28 @@
       <c r="E49" s="14">
         <v>32</v>
       </c>
+      <c r="G49" s="14">
+        <v>28</v>
+      </c>
+      <c r="H49" s="14">
+        <v>28</v>
+      </c>
       <c r="I49" s="22"/>
-      <c r="J49" s="2">
-        <v>1</v>
-      </c>
-      <c r="K49" s="2">
+      <c r="J49" s="36">
+        <v>1</v>
+      </c>
+      <c r="K49" s="36">
+        <v>1</v>
+      </c>
+      <c r="L49" s="2">
+        <v>1</v>
+      </c>
+      <c r="M49" s="2">
         <v>0.7</v>
       </c>
-      <c r="M49" s="34"/>
-      <c r="O49" s="85"/>
+      <c r="O49" s="34"/>
       <c r="P49" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L49:O49)</f>
         <v>1.7</v>
       </c>
       <c r="Q49" s="15"/>
@@ -3655,7 +3990,7 @@
     <row r="50" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C50" s="14">
         <v>4</v>
@@ -3665,21 +4000,29 @@
         <v>33</v>
       </c>
       <c r="F50" s="14"/>
-      <c r="G50" s="14"/>
-      <c r="H50" s="14"/>
+      <c r="G50" s="14">
+        <v>29</v>
+      </c>
+      <c r="H50" s="14">
+        <v>29</v>
+      </c>
       <c r="I50" s="22"/>
-      <c r="J50" s="2">
-        <v>1</v>
-      </c>
-      <c r="K50" s="2">
-        <v>1</v>
-      </c>
-      <c r="L50" s="20"/>
-      <c r="M50" s="34"/>
-      <c r="N50" s="2"/>
-      <c r="O50" s="85"/>
+      <c r="J50" s="36">
+        <v>1</v>
+      </c>
+      <c r="K50" s="36">
+        <v>1</v>
+      </c>
+      <c r="L50" s="2">
+        <v>1</v>
+      </c>
+      <c r="M50" s="2">
+        <v>1</v>
+      </c>
+      <c r="N50" s="20"/>
+      <c r="O50" s="34"/>
       <c r="P50" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L50:O50)</f>
         <v>2</v>
       </c>
       <c r="Q50" s="15"/>
@@ -3694,19 +4037,21 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C51" s="14">
         <v>3</v>
       </c>
       <c r="I51" s="22"/>
-      <c r="K51" s="2">
-        <v>0</v>
-      </c>
-      <c r="M51" s="34"/>
-      <c r="O51" s="85"/>
+      <c r="K51" s="36">
+        <v>0.5</v>
+      </c>
+      <c r="M51" s="2">
+        <v>0</v>
+      </c>
+      <c r="O51" s="34"/>
       <c r="P51" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L51:O51)</f>
         <v>0</v>
       </c>
       <c r="Q51" s="15"/>
@@ -3714,19 +4059,18 @@
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C52" s="14">
         <v>4</v>
       </c>
       <c r="I52" s="22"/>
-      <c r="K52" s="2">
-        <v>0</v>
-      </c>
-      <c r="M52" s="34"/>
-      <c r="O52" s="85"/>
+      <c r="M52" s="2">
+        <v>0</v>
+      </c>
+      <c r="O52" s="34"/>
       <c r="P52" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L52:O52)</f>
         <v>0</v>
       </c>
       <c r="Q52" s="15"/>
@@ -3734,7 +4078,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C53" s="14">
         <v>6</v>
@@ -3742,14 +4086,16 @@
       <c r="E53" s="14">
         <v>34</v>
       </c>
+      <c r="H53" s="14">
+        <v>30</v>
+      </c>
       <c r="I53" s="22"/>
-      <c r="K53" s="2">
+      <c r="M53" s="2">
         <v>0.7</v>
       </c>
-      <c r="M53" s="34"/>
-      <c r="O53" s="33"/>
+      <c r="O53" s="34"/>
       <c r="P53" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L53:O53)</f>
         <v>0.7</v>
       </c>
       <c r="Q53" s="15"/>
@@ -3758,7 +4104,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C54" s="14">
         <v>3</v>
@@ -3766,17 +4112,28 @@
       <c r="E54" s="14">
         <v>35</v>
       </c>
+      <c r="G54" s="14">
+        <v>30</v>
+      </c>
+      <c r="H54" s="14">
+        <v>31</v>
+      </c>
       <c r="I54" s="22"/>
-      <c r="J54" s="2">
-        <v>1</v>
-      </c>
-      <c r="K54" s="2">
-        <v>1</v>
-      </c>
-      <c r="M54" s="34"/>
-      <c r="O54" s="33"/>
+      <c r="J54" s="36">
+        <v>1</v>
+      </c>
+      <c r="K54" s="36">
+        <v>1</v>
+      </c>
+      <c r="L54" s="2">
+        <v>1</v>
+      </c>
+      <c r="M54" s="2">
+        <v>1</v>
+      </c>
+      <c r="O54" s="34"/>
       <c r="P54" s="77">
-        <f t="shared" si="0"/>
+        <f>SUM(L54:O54)</f>
         <v>2</v>
       </c>
       <c r="Q54" s="15"/>
@@ -3787,7 +4144,7 @@
         <v>117</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C55" s="13">
         <v>2</v>
@@ -3797,19 +4154,25 @@
         <v>36</v>
       </c>
       <c r="F55" s="13"/>
-      <c r="G55" s="13"/>
-      <c r="H55" s="13"/>
+      <c r="G55" s="13">
+        <v>31</v>
+      </c>
+      <c r="H55" s="13">
+        <v>32</v>
+      </c>
       <c r="I55" s="21"/>
-      <c r="J55" s="12"/>
-      <c r="K55" s="12">
+      <c r="J55" s="35"/>
+      <c r="K55" s="35">
         <v>1</v>
       </c>
       <c r="L55" s="12"/>
-      <c r="M55" s="35"/>
+      <c r="M55" s="12">
+        <v>1</v>
+      </c>
       <c r="N55" s="12"/>
       <c r="O55" s="35"/>
       <c r="P55" s="78">
-        <f t="shared" ref="P55:P67" si="2">SUM(J55:O55)</f>
+        <f>SUM(L55:O55)</f>
         <v>1</v>
       </c>
       <c r="Q55" s="15"/>
@@ -3818,7 +4181,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="C56" s="14">
         <v>7</v>
@@ -3826,17 +4189,28 @@
       <c r="E56" s="14">
         <v>37</v>
       </c>
+      <c r="G56" s="14">
+        <v>32</v>
+      </c>
+      <c r="H56" s="14">
+        <v>33</v>
+      </c>
       <c r="I56" s="22"/>
-      <c r="J56" s="2">
-        <v>1</v>
-      </c>
-      <c r="K56" s="2">
-        <v>1</v>
-      </c>
-      <c r="M56" s="34"/>
-      <c r="O56" s="33"/>
+      <c r="J56" s="36">
+        <v>1</v>
+      </c>
+      <c r="K56" s="36">
+        <v>1</v>
+      </c>
+      <c r="L56" s="2">
+        <v>1</v>
+      </c>
+      <c r="M56" s="2">
+        <v>1</v>
+      </c>
+      <c r="O56" s="34"/>
       <c r="P56" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L56:O56)</f>
         <v>2</v>
       </c>
       <c r="Q56" s="15"/>
@@ -3844,7 +4218,7 @@
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C57" s="14">
         <v>2</v>
@@ -3852,17 +4226,28 @@
       <c r="E57" s="14">
         <v>38</v>
       </c>
+      <c r="G57" s="14">
+        <v>33</v>
+      </c>
+      <c r="H57" s="14">
+        <v>34</v>
+      </c>
       <c r="I57" s="22"/>
-      <c r="J57" s="2">
-        <v>1</v>
-      </c>
-      <c r="K57" s="2">
-        <v>1</v>
-      </c>
-      <c r="M57" s="34"/>
-      <c r="O57" s="33"/>
+      <c r="J57" s="36">
+        <v>1</v>
+      </c>
+      <c r="K57" s="36">
+        <v>1</v>
+      </c>
+      <c r="L57" s="2">
+        <v>1</v>
+      </c>
+      <c r="M57" s="2">
+        <v>1</v>
+      </c>
+      <c r="O57" s="34"/>
       <c r="P57" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L57:O57)</f>
         <v>2</v>
       </c>
       <c r="Q57" s="15"/>
@@ -3873,19 +4258,18 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="C58" s="14">
         <v>3</v>
       </c>
       <c r="I58" s="22"/>
-      <c r="K58" s="2">
-        <v>0</v>
-      </c>
-      <c r="M58" s="34"/>
+      <c r="M58" s="2">
+        <v>0</v>
+      </c>
       <c r="O58" s="34"/>
       <c r="P58" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L58:O58)</f>
         <v>0</v>
       </c>
       <c r="Q58" s="15"/>
@@ -3896,7 +4280,7 @@
         <v>116</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C59" s="13">
         <v>4</v>
@@ -3909,16 +4293,18 @@
       <c r="G59" s="13"/>
       <c r="H59" s="13"/>
       <c r="I59" s="21"/>
-      <c r="J59" s="12"/>
-      <c r="K59" s="12">
-        <v>0</v>
-      </c>
+      <c r="J59" s="35">
+        <v>1</v>
+      </c>
+      <c r="K59" s="35"/>
       <c r="L59" s="12"/>
-      <c r="M59" s="35"/>
+      <c r="M59" s="12">
+        <v>0</v>
+      </c>
       <c r="N59" s="12"/>
       <c r="O59" s="35"/>
       <c r="P59" s="78">
-        <f t="shared" si="2"/>
+        <f>SUM(L59:O59)</f>
         <v>0</v>
       </c>
       <c r="Q59" s="15"/>
@@ -3927,7 +4313,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C60" s="14">
         <v>3</v>
@@ -3936,13 +4322,15 @@
         <v>40</v>
       </c>
       <c r="I60" s="22"/>
-      <c r="K60" s="2">
-        <v>0</v>
-      </c>
-      <c r="M60" s="34"/>
-      <c r="O60" s="33"/>
+      <c r="J60" s="36">
+        <v>1</v>
+      </c>
+      <c r="M60" s="2">
+        <v>0</v>
+      </c>
+      <c r="O60" s="34"/>
       <c r="P60" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L60:O60)</f>
         <v>0</v>
       </c>
       <c r="Q60" s="15"/>
@@ -3966,18 +4354,18 @@
       <c r="G61" s="13"/>
       <c r="H61" s="13"/>
       <c r="I61" s="21"/>
-      <c r="J61" s="12">
-        <v>1</v>
-      </c>
-      <c r="K61" s="12">
-        <v>1</v>
-      </c>
-      <c r="L61" s="12"/>
-      <c r="M61" s="35"/>
+      <c r="J61" s="35"/>
+      <c r="K61" s="35"/>
+      <c r="L61" s="12">
+        <v>1</v>
+      </c>
+      <c r="M61" s="12">
+        <v>1</v>
+      </c>
       <c r="N61" s="12"/>
       <c r="O61" s="35"/>
       <c r="P61" s="78">
-        <f t="shared" si="2"/>
+        <f>SUM(L61:O61)</f>
         <v>2</v>
       </c>
       <c r="Q61" s="15"/>
@@ -3994,15 +4382,13 @@
         <v>1</v>
       </c>
       <c r="I62" s="22"/>
-      <c r="J62" s="20"/>
-      <c r="K62" s="20">
-        <v>1</v>
-      </c>
-      <c r="M62" s="36"/>
-      <c r="N62" s="20"/>
+      <c r="L62" s="20"/>
+      <c r="M62" s="20">
+        <v>1</v>
+      </c>
       <c r="O62" s="36"/>
       <c r="P62" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L62:O62)</f>
         <v>1</v>
       </c>
       <c r="Q62" s="15"/>
@@ -4023,18 +4409,18 @@
       <c r="G63" s="14"/>
       <c r="H63" s="14"/>
       <c r="I63" s="22"/>
-      <c r="J63" s="2">
-        <v>1</v>
-      </c>
-      <c r="K63" s="2">
-        <v>1</v>
-      </c>
-      <c r="L63" s="20"/>
-      <c r="M63" s="34"/>
-      <c r="N63" s="2"/>
-      <c r="O63" s="33"/>
+      <c r="J63" s="36"/>
+      <c r="K63" s="36"/>
+      <c r="L63" s="2">
+        <v>1</v>
+      </c>
+      <c r="M63" s="2">
+        <v>1</v>
+      </c>
+      <c r="N63" s="20"/>
+      <c r="O63" s="34"/>
       <c r="P63" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L63:O63)</f>
         <v>2</v>
       </c>
       <c r="Q63" s="15"/>
@@ -4058,16 +4444,15 @@
         <v>3</v>
       </c>
       <c r="I64" s="22"/>
-      <c r="J64" s="2">
-        <v>1</v>
-      </c>
-      <c r="K64" s="2">
-        <v>1</v>
-      </c>
-      <c r="M64" s="34"/>
-      <c r="O64" s="33"/>
+      <c r="L64" s="2">
+        <v>1</v>
+      </c>
+      <c r="M64" s="2">
+        <v>1</v>
+      </c>
+      <c r="O64" s="34"/>
       <c r="P64" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L64:O64)</f>
         <v>2</v>
       </c>
       <c r="Q64" s="15"/>
@@ -4087,13 +4472,15 @@
       <c r="I65" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="K65" s="2">
-        <v>0</v>
-      </c>
-      <c r="M65" s="34"/>
-      <c r="O65" s="33"/>
+      <c r="K65" s="36">
+        <v>1</v>
+      </c>
+      <c r="M65" s="2">
+        <v>0</v>
+      </c>
+      <c r="O65" s="34"/>
       <c r="P65" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L65:O65)</f>
         <v>0</v>
       </c>
       <c r="Q65" s="15"/>
@@ -4113,16 +4500,15 @@
         <v>1</v>
       </c>
       <c r="I66" s="22"/>
-      <c r="J66" s="2">
-        <v>1</v>
-      </c>
-      <c r="K66" s="2">
-        <v>1</v>
-      </c>
-      <c r="M66" s="34"/>
-      <c r="O66" s="33"/>
+      <c r="L66" s="2">
+        <v>1</v>
+      </c>
+      <c r="M66" s="2">
+        <v>1</v>
+      </c>
+      <c r="O66" s="34"/>
       <c r="P66" s="77">
-        <f t="shared" si="2"/>
+        <f>SUM(L66:O66)</f>
         <v>2</v>
       </c>
       <c r="Q66" s="15"/>
@@ -4143,18 +4529,18 @@
       <c r="G67" s="27"/>
       <c r="H67" s="27"/>
       <c r="I67" s="29"/>
-      <c r="J67" s="28">
-        <v>1</v>
-      </c>
-      <c r="K67" s="28">
-        <v>0</v>
-      </c>
-      <c r="L67" s="28"/>
-      <c r="M67" s="37"/>
+      <c r="J67" s="37"/>
+      <c r="K67" s="37"/>
+      <c r="L67" s="28">
+        <v>1</v>
+      </c>
+      <c r="M67" s="28">
+        <v>0</v>
+      </c>
       <c r="N67" s="28"/>
       <c r="O67" s="37"/>
       <c r="P67" s="79">
-        <f t="shared" si="2"/>
+        <f>SUM(L67:O67)</f>
         <v>1</v>
       </c>
       <c r="Q67" s="15"/>
@@ -4175,21 +4561,15 @@
       <c r="I69" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J69" s="65">
-        <f t="array" ref="J69">SUM($C2:$C67*(J2:J67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>178</v>
-      </c>
-      <c r="K69" s="65">
-        <f t="array" ref="K69">SUM($C2:$C67*(K2:K67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>110</v>
-      </c>
+      <c r="J69" s="85"/>
+      <c r="K69" s="85"/>
       <c r="L69" s="65">
         <f t="array" ref="L69">SUM($C2:$C67*(L2:L67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>178</v>
       </c>
       <c r="M69" s="65">
         <f t="array" ref="M69">SUM($C2:$C67*(M2:M67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>110</v>
       </c>
       <c r="N69" s="65">
         <f t="array" ref="N69">SUM($C2:$C67*(N2:N67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
@@ -4206,21 +4586,15 @@
       <c r="I70" s="67" t="s">
         <v>100</v>
       </c>
-      <c r="J70" s="68">
-        <f t="array" ref="J70">SUM($C2:$C67*J2:J67*($P2:$P67&gt;=$R$12))</f>
-        <v>180.5</v>
-      </c>
-      <c r="K70" s="68">
-        <f t="array" ref="K70">SUM($C2:$C67*K2:K67*($P2:$P67&gt;=$R$12))</f>
-        <v>154.80000000000001</v>
-      </c>
+      <c r="J70" s="86"/>
+      <c r="K70" s="86"/>
       <c r="L70" s="68">
         <f t="array" ref="L70">SUM($C2:$C67*L2:L67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>180.5</v>
       </c>
       <c r="M70" s="68">
         <f t="array" ref="M70">SUM($C2:$C67*M2:M67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>154.80000000000001</v>
       </c>
       <c r="N70" s="68">
         <f t="array" ref="N70">SUM($C2:$C67*N2:N67*($P2:$P67&gt;=$R$12))</f>
@@ -4240,21 +4614,15 @@
       <c r="I71" s="67" t="s">
         <v>99</v>
       </c>
-      <c r="J71" s="68">
-        <f t="array" ref="J71">SUM($C$2:$C$67*(J$2:J$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>183</v>
-      </c>
-      <c r="K71" s="68">
-        <f t="array" ref="K71">SUM($C$2:$C$67*(K$2:K$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>183</v>
-      </c>
+      <c r="J71" s="86"/>
+      <c r="K71" s="86"/>
       <c r="L71" s="68">
         <f t="array" ref="L71">SUM($C$2:$C$67*(L$2:L$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="M71" s="68">
         <f t="array" ref="M71">SUM($C$2:$C$67*(M$2:M$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>0</v>
+        <v>183</v>
       </c>
       <c r="N71" s="68">
         <f t="array" ref="N71">SUM($C$2:$C$67*(N$2:N$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
@@ -4278,28 +4646,22 @@
       <c r="I72" s="67" t="s">
         <v>101</v>
       </c>
-      <c r="J72" s="68">
-        <f t="shared" ref="J72:O72" si="3">LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+      <c r="J72" s="86"/>
+      <c r="K72" s="86"/>
+      <c r="L72" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>183</v>
       </c>
-      <c r="K72" s="68">
-        <f t="shared" si="3"/>
+      <c r="M72" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>183</v>
       </c>
-      <c r="L72" s="68">
-        <f t="shared" si="3"/>
+      <c r="N72" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>183</v>
       </c>
-      <c r="M72" s="68">
-        <f t="shared" si="3"/>
-        <v>183</v>
-      </c>
-      <c r="N72" s="68">
-        <f t="shared" si="3"/>
-        <v>183</v>
-      </c>
       <c r="O72" s="69">
-        <f t="shared" si="3"/>
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
         <v>183</v>
       </c>
       <c r="P72" s="3"/>
@@ -4317,28 +4679,22 @@
       <c r="I73" s="67" t="s">
         <v>102</v>
       </c>
-      <c r="J73" s="70">
-        <f t="shared" ref="J73:O73" si="4">J70/J72</f>
+      <c r="J73" s="86"/>
+      <c r="K73" s="86"/>
+      <c r="L73" s="70">
+        <f t="shared" ref="L73:O73" si="1">L70/L72</f>
         <v>0.98633879781420764</v>
       </c>
-      <c r="K73" s="70">
-        <f t="shared" si="4"/>
+      <c r="M73" s="70">
+        <f t="shared" si="1"/>
         <v>0.84590163934426232</v>
       </c>
-      <c r="L73" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="M73" s="70">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
       <c r="N73" s="70">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="O73" s="71">
-        <f t="shared" si="4"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="Q73" s="15"/>
@@ -4352,21 +4708,15 @@
       <c r="I74" s="72" t="s">
         <v>80</v>
       </c>
-      <c r="J74" s="73">
-        <f t="array" ref="J74">SUM($C2:$C67*J2:J67*($P2:$P67&lt;$R$12))</f>
-        <v>15.5</v>
-      </c>
-      <c r="K74" s="73">
-        <f t="array" ref="K74">SUM($C2:$C67*K2:K67*($P2:$P67&lt;$R$12))</f>
-        <v>36.299999999999997</v>
-      </c>
+      <c r="J74" s="87"/>
+      <c r="K74" s="87"/>
       <c r="L74" s="73">
         <f t="array" ref="L74">SUM($C2:$C67*L2:L67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
+        <v>15.5</v>
       </c>
       <c r="M74" s="73">
         <f t="array" ref="M74">SUM($C2:$C67*M2:M67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
+        <v>36.299999999999997</v>
       </c>
       <c r="N74" s="73">
         <f t="array" ref="N74">SUM($C2:$C67*N2:N67*($P2:$P67&lt;$R$12))</f>
@@ -4391,6 +4741,8 @@
       <c r="I76" s="14"/>
       <c r="J76" s="14"/>
       <c r="K76" s="14"/>
+      <c r="L76" s="14"/>
+      <c r="M76" s="14"/>
       <c r="Q76" s="15"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.3">
@@ -4398,24 +4750,32 @@
       <c r="I77" s="14"/>
       <c r="J77" s="14"/>
       <c r="K77" s="14"/>
+      <c r="L77" s="14"/>
+      <c r="M77" s="14"/>
       <c r="Q77" s="15"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="14"/>
+      <c r="L78" s="14"/>
+      <c r="M78" s="14"/>
       <c r="Q78" s="15"/>
     </row>
     <row r="79" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I79" s="14"/>
       <c r="J79" s="14"/>
       <c r="K79" s="14"/>
+      <c r="L79" s="14"/>
+      <c r="M79" s="14"/>
       <c r="Q79" s="15"/>
     </row>
     <row r="80" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I80" s="14"/>
       <c r="J80" s="14"/>
       <c r="K80" s="14"/>
+      <c r="L80" s="14"/>
+      <c r="M80" s="14"/>
       <c r="Q80" s="15"/>
       <c r="U80" s="33"/>
     </row>
@@ -4423,17 +4783,23 @@
       <c r="I81" s="14"/>
       <c r="J81" s="14"/>
       <c r="K81" s="14"/>
+      <c r="L81" s="14"/>
+      <c r="M81" s="14"/>
       <c r="Q81" s="15"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I82" s="14"/>
       <c r="J82" s="14"/>
       <c r="K82" s="14"/>
+      <c r="L82" s="14"/>
+      <c r="M82" s="14"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I83" s="14"/>
       <c r="J83" s="14"/>
       <c r="K83" s="14"/>
+      <c r="L83" s="14"/>
+      <c r="M83" s="14"/>
     </row>
     <row r="85" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A85" s="10"/>
@@ -4445,11 +4811,11 @@
       <c r="G85" s="14"/>
       <c r="H85" s="14"/>
       <c r="I85" s="20"/>
-      <c r="J85" s="2"/>
-      <c r="K85" s="2"/>
-      <c r="L85" s="20"/>
+      <c r="J85" s="36"/>
+      <c r="K85" s="36"/>
+      <c r="L85" s="2"/>
       <c r="M85" s="2"/>
-      <c r="N85" s="2"/>
+      <c r="N85" s="20"/>
       <c r="O85" s="2"/>
       <c r="P85" s="3"/>
       <c r="Q85" s="3"/>
@@ -4488,13 +4854,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="B2:P67">
-    <cfRule type="expression" dxfId="2" priority="28" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="31" stopIfTrue="1">
       <formula>$P2&gt;=(0.5+$R$12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="29" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="32" stopIfTrue="1">
       <formula>$P2&gt;=$R$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="30">
+    <cfRule type="expression" dxfId="12" priority="33">
       <formula>$P2&gt;=($R$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Updated master.tex for fall 2017, draft version
</commit_message>
<xml_diff>
--- a/StudentGuideModule1/what_labs_to_include/131 lab list for 2017fall.xlsx
+++ b/StudentGuideModule1/what_labs_to_include/131 lab list for 2017fall.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Box Sync\teaching\_phy132_2017\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mtrawick\Desktop\github\131\StudentGuideModule1\what_labs_to_include\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="192" windowWidth="22980" windowHeight="9408" tabRatio="541"/>
+    <workbookView xWindow="0" yWindow="192" windowWidth="22980" windowHeight="9408" tabRatio="539"/>
   </bookViews>
   <sheets>
     <sheet name="lablist" sheetId="1" r:id="rId1"/>
@@ -180,7 +180,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="183">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="184">
   <si>
     <t>1 Music to Our Ears: Standing Waves in Strings 7</t>
   </si>
@@ -492,10 +492,6 @@
     <t>expected percent of manual used</t>
   </si>
   <si>
-    <t># users 
-for 2017</t>
-  </si>
-  <si>
     <t># of users</t>
   </si>
   <si>
@@ -523,14 +519,6 @@
     <t>lab# fa15</t>
   </si>
   <si>
-    <t>2017 
-Henry</t>
-  </si>
-  <si>
-    <t>2017 
-Con</t>
-  </si>
-  <si>
     <t>New by Ted 2015</t>
   </si>
   <si>
@@ -715,9 +703,6 @@
   </si>
   <si>
     <t>The Twins Paradox</t>
-  </si>
-  <si>
-    <t>2017 Mariama</t>
   </si>
   <si>
     <t>Equations to Define Velocity and Acceleration</t>
@@ -733,8 +718,24 @@
     <t>2016 fall Christine</t>
   </si>
   <si>
-    <t>2017 
-Dr. Staff</t>
+    <t>2017 spr
+Henry</t>
+  </si>
+  <si>
+    <t>2017 spr
+Con</t>
+  </si>
+  <si>
+    <t>2017 sum Alina</t>
+  </si>
+  <si>
+    <t>ipads</t>
+  </si>
+  <si>
+    <t>Force by Matt</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># users </t>
   </si>
 </sst>
 </file>
@@ -1618,91 +1619,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="15">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFFF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFCDFFCD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF99"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill>
@@ -2033,10 +1950,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y110"/>
+  <dimension ref="A1:Y111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B55" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P78" sqref="P78"/>
+    <sheetView tabSelected="1" topLeftCell="A46" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R66" sqref="R66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2058,7 +1975,7 @@
     <col min="21" max="21" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="48" t="s">
         <v>73</v>
       </c>
@@ -2072,40 +1989,40 @@
         <v>76</v>
       </c>
       <c r="E1" s="50" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F1" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="G1" s="50" t="s">
         <v>108</v>
       </c>
-      <c r="G1" s="50" t="s">
+      <c r="H1" s="50" t="s">
         <v>109</v>
-      </c>
-      <c r="H1" s="50" t="s">
-        <v>110</v>
       </c>
       <c r="I1" s="51" t="s">
         <v>90</v>
       </c>
       <c r="J1" s="49" t="s">
+        <v>176</v>
+      </c>
+      <c r="K1" s="49" t="s">
+        <v>177</v>
+      </c>
+      <c r="L1" s="49" t="s">
+        <v>178</v>
+      </c>
+      <c r="M1" s="49" t="s">
+        <v>179</v>
+      </c>
+      <c r="N1" s="49" t="s">
         <v>180</v>
-      </c>
-      <c r="K1" s="49" t="s">
-        <v>181</v>
-      </c>
-      <c r="L1" s="49" t="s">
-        <v>113</v>
-      </c>
-      <c r="M1" s="49" t="s">
-        <v>114</v>
-      </c>
-      <c r="N1" s="49" t="s">
-        <v>177</v>
       </c>
       <c r="O1" s="49" t="s">
         <v>182</v>
       </c>
       <c r="P1" s="52" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="Q1" s="32"/>
       <c r="R1" s="33"/>
@@ -2148,8 +2065,8 @@
       <c r="N2" s="59"/>
       <c r="O2" s="55"/>
       <c r="P2" s="75">
-        <f>SUM(L2:O2)</f>
-        <v>2</v>
+        <f>SUM(J2:O2)</f>
+        <v>3</v>
       </c>
       <c r="Q2" s="80"/>
       <c r="R2" s="80"/>
@@ -2190,8 +2107,8 @@
       <c r="N3" s="60"/>
       <c r="O3" s="60"/>
       <c r="P3" s="76">
-        <f>SUM(L3:O3)</f>
-        <v>2</v>
+        <f t="shared" ref="P3:P67" si="0">SUM(J3:O3)</f>
+        <v>3</v>
       </c>
       <c r="Q3" s="80"/>
       <c r="R3" s="80"/>
@@ -2205,10 +2122,10 @@
     </row>
     <row r="4" spans="1:25" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="30" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B4" s="23" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C4" s="14">
         <v>4</v>
@@ -2235,11 +2152,13 @@
       <c r="M4" s="36">
         <v>0.5</v>
       </c>
-      <c r="N4" s="36"/>
+      <c r="N4" s="36">
+        <v>1</v>
+      </c>
       <c r="O4" s="36"/>
       <c r="P4" s="77">
-        <f>SUM(L4:O4)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>3.5</v>
       </c>
       <c r="Q4" s="5"/>
       <c r="R4" s="5"/>
@@ -2253,7 +2172,7 @@
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="C5" s="14">
         <v>1</v>
@@ -2267,7 +2186,7 @@
       </c>
       <c r="O5" s="34"/>
       <c r="P5" s="77">
-        <f>SUM(L5:O5)</f>
+        <f t="shared" si="0"/>
         <v>0.75</v>
       </c>
       <c r="Q5" s="5"/>
@@ -2283,7 +2202,7 @@
     <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="30"/>
       <c r="B6" s="31" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C6" s="14">
         <v>2</v>
@@ -2296,7 +2215,7 @@
       <c r="N6" s="36"/>
       <c r="O6" s="36"/>
       <c r="P6" s="77">
-        <f>SUM(L6:O6)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q6" s="5"/>
@@ -2312,7 +2231,7 @@
     <row r="7" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="10"/>
       <c r="B7" s="23" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="C7" s="14">
         <v>2</v>
@@ -2332,7 +2251,7 @@
       <c r="N7" s="20"/>
       <c r="O7" s="34"/>
       <c r="P7" s="77">
-        <f>SUM(L7:O7)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q7" s="5"/>
@@ -2343,7 +2262,7 @@
     </row>
     <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B8" s="23" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="C8" s="14">
         <v>2</v>
@@ -2354,7 +2273,7 @@
       </c>
       <c r="O8" s="34"/>
       <c r="P8" s="77">
-        <f>SUM(L8:O8)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q8" s="5"/>
@@ -2369,7 +2288,7 @@
     </row>
     <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B9" s="23" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C9" s="14">
         <v>7</v>
@@ -2396,10 +2315,13 @@
       <c r="M9" s="2">
         <v>1</v>
       </c>
+      <c r="N9" s="20">
+        <v>1</v>
+      </c>
       <c r="O9" s="34"/>
       <c r="P9" s="77">
-        <f>SUM(L9:O9)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q9" s="5"/>
       <c r="R9" s="5"/>
@@ -2413,7 +2335,7 @@
     </row>
     <row r="10" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="23" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C10" s="14">
         <v>8</v>
@@ -2440,11 +2362,13 @@
       <c r="M10" s="34">
         <v>1</v>
       </c>
-      <c r="N10" s="36"/>
+      <c r="N10" s="36">
+        <v>1</v>
+      </c>
       <c r="O10" s="34"/>
       <c r="P10" s="77">
-        <f>SUM(L10:O10)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q10" s="5"/>
       <c r="R10" s="5"/>
@@ -2458,7 +2382,7 @@
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C11" s="14">
         <v>5</v>
@@ -2482,11 +2406,13 @@
       <c r="M11" s="34">
         <v>0.75</v>
       </c>
-      <c r="N11" s="36"/>
+      <c r="N11" s="36">
+        <v>1</v>
+      </c>
       <c r="O11" s="34"/>
       <c r="P11" s="77">
-        <f>SUM(L11:O11)</f>
-        <v>1.75</v>
+        <f t="shared" si="0"/>
+        <v>3.25</v>
       </c>
       <c r="Q11" s="5"/>
       <c r="R11" s="42" t="s">
@@ -2502,7 +2428,7 @@
     </row>
     <row r="12" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="23" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C12" s="14">
         <v>3</v>
@@ -2518,8 +2444,8 @@
       <c r="N12" s="36"/>
       <c r="O12" s="34"/>
       <c r="P12" s="77">
-        <f>SUM(L12:O12)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="Q12" s="15"/>
       <c r="R12" s="44">
@@ -2535,7 +2461,7 @@
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="C13" s="14">
         <v>12</v>
@@ -2559,11 +2485,13 @@
       <c r="M13" s="34">
         <v>1</v>
       </c>
-      <c r="N13" s="36"/>
+      <c r="N13" s="36">
+        <v>1</v>
+      </c>
       <c r="O13" s="34"/>
       <c r="P13" s="77">
-        <f>SUM(L13:O13)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q13" s="5"/>
       <c r="R13" s="33"/>
@@ -2577,7 +2505,7 @@
     </row>
     <row r="14" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="23" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C14" s="14">
         <v>13</v>
@@ -2601,11 +2529,13 @@
       <c r="M14" s="34">
         <v>0.5</v>
       </c>
-      <c r="N14" s="36"/>
+      <c r="N14" s="36">
+        <v>1</v>
+      </c>
       <c r="O14" s="34"/>
       <c r="P14" s="77">
-        <f>SUM(L14:O14)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>3.5</v>
       </c>
       <c r="Q14" s="5"/>
       <c r="R14" s="1" t="s">
@@ -2620,7 +2550,7 @@
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C15" s="14">
         <v>6</v>
@@ -2636,7 +2566,7 @@
       <c r="N15" s="36"/>
       <c r="O15" s="34"/>
       <c r="P15" s="77">
-        <f>SUM(L15:O15)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q15" s="5"/>
@@ -2655,7 +2585,7 @@
     </row>
     <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C16" s="14">
         <v>3</v>
@@ -2671,8 +2601,8 @@
       <c r="N16" s="36"/>
       <c r="O16" s="34"/>
       <c r="P16" s="77">
-        <f>SUM(L16:O16)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="Q16" s="5"/>
       <c r="R16" s="18" t="s">
@@ -2690,7 +2620,7 @@
     </row>
     <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C17" s="14">
         <v>5</v>
@@ -2706,10 +2636,12 @@
         <v>0.75</v>
       </c>
       <c r="N17" s="36"/>
-      <c r="O17" s="34"/>
+      <c r="O17" s="34">
+        <v>1</v>
+      </c>
       <c r="P17" s="77">
-        <f>SUM(L17:O17)</f>
-        <v>1.25</v>
+        <f t="shared" si="0"/>
+        <v>2.25</v>
       </c>
       <c r="Q17" s="5"/>
       <c r="R17" s="18" t="s">
@@ -2727,7 +2659,7 @@
     </row>
     <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B18" s="23" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C18" s="14">
         <v>3</v>
@@ -2754,11 +2686,13 @@
       <c r="M18" s="34">
         <v>0.75</v>
       </c>
-      <c r="N18" s="36"/>
+      <c r="N18" s="36">
+        <v>1</v>
+      </c>
       <c r="O18" s="34"/>
       <c r="P18" s="77">
-        <f>SUM(L18:O18)</f>
-        <v>1.75</v>
+        <f t="shared" si="0"/>
+        <v>4.75</v>
       </c>
       <c r="Q18" s="5"/>
       <c r="R18" s="18" t="s">
@@ -2776,7 +2710,7 @@
     </row>
     <row r="19" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B19" s="23" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C19" s="14">
         <v>2</v>
@@ -2789,7 +2723,7 @@
       <c r="N19" s="36"/>
       <c r="O19" s="34"/>
       <c r="P19" s="77">
-        <f>SUM(L19:O19)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q19" s="15"/>
@@ -2808,7 +2742,7 @@
     </row>
     <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C20" s="14">
         <v>1</v>
@@ -2821,7 +2755,7 @@
       <c r="N20" s="36"/>
       <c r="O20" s="34"/>
       <c r="P20" s="77">
-        <f>SUM(L20:O20)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q20" s="15"/>
@@ -2833,7 +2767,7 @@
     </row>
     <row r="21" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="23" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C21" s="14">
         <v>2</v>
@@ -2846,7 +2780,7 @@
       <c r="N21" s="36"/>
       <c r="O21" s="34"/>
       <c r="P21" s="77">
-        <f>SUM(L21:O21)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q21" s="15"/>
@@ -2861,7 +2795,7 @@
     </row>
     <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C22" s="14">
         <v>1</v>
@@ -2875,21 +2809,21 @@
       </c>
       <c r="O22" s="34"/>
       <c r="P22" s="77">
-        <f>SUM(L22:O22)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="Q22" s="15"/>
       <c r="R22" s="46" t="s">
+        <v>103</v>
+      </c>
+      <c r="S22" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="S22" s="4" t="s">
+      <c r="T22" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="T22" s="4" t="s">
+      <c r="U22" s="7" t="s">
         <v>106</v>
-      </c>
-      <c r="U22" s="7" t="s">
-        <v>107</v>
       </c>
       <c r="V22" s="33"/>
       <c r="W22" s="33"/>
@@ -2898,7 +2832,7 @@
     </row>
     <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B23" s="23" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C23" s="14">
         <v>2</v>
@@ -2909,7 +2843,7 @@
       </c>
       <c r="O23" s="34"/>
       <c r="P23" s="77">
-        <f>SUM(L23:O23)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q23" s="15"/>
@@ -2917,15 +2851,15 @@
         <v>0</v>
       </c>
       <c r="S23" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R23,C$2:C$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R23,C$2:C$69)</f>
         <v>296</v>
       </c>
       <c r="T23" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R23,D$2:D$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R23,D$2:D$69)</f>
         <v>7</v>
       </c>
       <c r="U23" s="8">
-        <f t="shared" ref="U23:U31" si="0">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
+        <f t="shared" ref="U23:U31" si="1">($T$17 + $T$15*S23+$T$16*T23)*(1+T$18+T$19)</f>
         <v>25.870000000000005</v>
       </c>
       <c r="V23" s="33"/>
@@ -2936,7 +2870,7 @@
     <row r="24" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="10"/>
       <c r="B24" s="23" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C24" s="14">
         <v>3</v>
@@ -2965,27 +2899,29 @@
       <c r="M24" s="2">
         <v>1</v>
       </c>
-      <c r="N24" s="20"/>
+      <c r="N24" s="20">
+        <v>1</v>
+      </c>
       <c r="O24" s="34"/>
       <c r="P24" s="77">
-        <f>SUM(L24:O24)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q24" s="15"/>
       <c r="R24" s="81">
         <v>0.5</v>
       </c>
       <c r="S24" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R24,C$2:C$68)</f>
-        <v>244</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R24,C$2:C$69)</f>
+        <v>268</v>
       </c>
       <c r="T24" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R24,D$2:D$68)</f>
-        <v>7</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R24,D$2:D$69)</f>
+        <v>6</v>
       </c>
       <c r="U24" s="8">
-        <f t="shared" si="0"/>
-        <v>22.490000000000002</v>
+        <f t="shared" si="1"/>
+        <v>23.66</v>
       </c>
       <c r="V24" s="33"/>
       <c r="W24" s="33"/>
@@ -2994,13 +2930,13 @@
     </row>
     <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C25" s="14">
         <v>4</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L25" s="2">
         <v>1</v>
@@ -3008,26 +2944,29 @@
       <c r="M25" s="2">
         <v>0</v>
       </c>
+      <c r="N25" s="20">
+        <v>1</v>
+      </c>
       <c r="O25" s="34"/>
       <c r="P25" s="77">
-        <f>SUM(L25:O25)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="Q25" s="15"/>
       <c r="R25" s="81">
         <v>1</v>
       </c>
       <c r="S25" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R25,C$2:C$68)</f>
-        <v>215</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R25,C$2:C$69)</f>
+        <v>244</v>
       </c>
       <c r="T25" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R25,D$2:D$68)</f>
-        <v>7</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R25,D$2:D$69)</f>
+        <v>6</v>
       </c>
       <c r="U25" s="8">
-        <f t="shared" si="0"/>
-        <v>20.605</v>
+        <f t="shared" si="1"/>
+        <v>22.1</v>
       </c>
       <c r="V25" s="33"/>
       <c r="W25" s="33"/>
@@ -3036,7 +2975,7 @@
     </row>
     <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C26" s="14">
         <v>6</v>
@@ -3060,26 +2999,29 @@
       <c r="M26" s="2">
         <v>1</v>
       </c>
+      <c r="N26" s="20">
+        <v>1</v>
+      </c>
       <c r="O26" s="34"/>
       <c r="P26" s="77">
-        <f>SUM(L26:O26)</f>
-        <v>2</v>
+        <f>SUM(J26:O26)</f>
+        <v>4</v>
       </c>
       <c r="Q26" s="15"/>
       <c r="R26" s="82">
         <v>1.5</v>
       </c>
       <c r="S26" s="31">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R26,C$2:C$68)</f>
-        <v>183</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R26,C$2:C$69)</f>
+        <v>223</v>
       </c>
       <c r="T26" s="31">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R26,D$2:D$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R26,D$2:D$69)</f>
         <v>6</v>
       </c>
       <c r="U26" s="8">
-        <f t="shared" si="0"/>
-        <v>18.134999999999998</v>
+        <f t="shared" si="1"/>
+        <v>20.734999999999999</v>
       </c>
       <c r="V26" s="33"/>
       <c r="W26" s="33"/>
@@ -3088,13 +3030,13 @@
     </row>
     <row r="27" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="C27" s="13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D27" s="13"/>
       <c r="E27" s="13">
@@ -3120,32 +3062,34 @@
       <c r="M27" s="12">
         <v>1</v>
       </c>
-      <c r="N27" s="12"/>
+      <c r="N27" s="12">
+        <v>1</v>
+      </c>
       <c r="O27" s="35"/>
       <c r="P27" s="78">
-        <f>SUM(L27:O27)</f>
-        <v>2</v>
+        <f>SUM(J27:O27)</f>
+        <v>4.5</v>
       </c>
       <c r="Q27" s="15"/>
       <c r="R27" s="81">
         <v>2</v>
       </c>
       <c r="S27" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R27,C$2:C$68)</f>
-        <v>105</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R27,C$2:C$69)</f>
+        <v>223</v>
       </c>
       <c r="T27" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R27,D$2:D$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R27,D$2:D$69)</f>
         <v>6</v>
       </c>
       <c r="U27" s="8">
-        <f t="shared" si="0"/>
-        <v>13.065000000000001</v>
+        <f t="shared" si="1"/>
+        <v>20.734999999999999</v>
       </c>
     </row>
     <row r="28" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C28" s="14">
         <v>8</v>
@@ -3166,31 +3110,34 @@
       <c r="M28" s="2">
         <v>0.8</v>
       </c>
+      <c r="N28" s="20">
+        <v>1</v>
+      </c>
       <c r="O28" s="34"/>
       <c r="P28" s="77">
-        <f>SUM(L28:O28)</f>
-        <v>1.8</v>
+        <f t="shared" si="0"/>
+        <v>2.8</v>
       </c>
       <c r="Q28" s="15"/>
       <c r="R28" s="81">
         <v>2.5</v>
       </c>
       <c r="S28" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R28,C$2:C$68)</f>
-        <v>0</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R28,C$2:C$69)</f>
+        <v>199</v>
       </c>
       <c r="T28" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R28,D$2:D$68)</f>
-        <v>0</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R28,D$2:D$69)</f>
+        <v>1</v>
       </c>
       <c r="U28" s="8">
-        <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>17.225000000000001</v>
       </c>
     </row>
     <row r="29" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B29" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C29" s="14">
         <v>7</v>
@@ -3204,7 +3151,7 @@
       </c>
       <c r="O29" s="34"/>
       <c r="P29" s="77">
-        <f>SUM(L29:O29)</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="Q29" s="15"/>
@@ -3212,21 +3159,21 @@
         <v>3</v>
       </c>
       <c r="S29" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R29,C$2:C$68)</f>
-        <v>0</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R29,C$2:C$69)</f>
+        <v>168</v>
       </c>
       <c r="T29" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R29,D$2:D$68)</f>
-        <v>0</v>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R29,D$2:D$69)</f>
+        <v>1</v>
       </c>
       <c r="U29" s="8">
-        <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>15.210000000000003</v>
       </c>
     </row>
     <row r="30" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B30" s="23" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="C30" s="14">
         <v>9</v>
@@ -3248,32 +3195,34 @@
       <c r="M30" s="34">
         <v>0.5</v>
       </c>
-      <c r="N30" s="36"/>
+      <c r="N30" s="36">
+        <v>1</v>
+      </c>
       <c r="O30" s="34"/>
       <c r="P30" s="77">
-        <f>SUM(L30:O30)</f>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="Q30" s="15"/>
       <c r="R30" s="81">
         <v>3.5</v>
       </c>
       <c r="S30" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R30,C$2:C$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R30,C$2:C$69)</f>
+        <v>149</v>
+      </c>
+      <c r="T30" s="6">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R30,D$2:D$69)</f>
         <v>0</v>
       </c>
-      <c r="T30" s="6">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R30,D$2:D$68)</f>
-        <v>0</v>
-      </c>
       <c r="U30" s="8">
-        <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>13.584999999999999</v>
       </c>
     </row>
     <row r="31" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="23" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C31" s="14">
         <v>7</v>
@@ -3300,33 +3249,35 @@
       <c r="M31" s="34">
         <v>0.5</v>
       </c>
-      <c r="N31" s="36"/>
+      <c r="N31" s="36">
+        <v>1</v>
+      </c>
       <c r="O31" s="34"/>
       <c r="P31" s="77">
-        <f>SUM(L31:O31)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
       <c r="Q31" s="15"/>
       <c r="R31" s="83">
         <v>4</v>
       </c>
       <c r="S31" s="47">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R31,C$2:C$68)</f>
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R31,C$2:C$69)</f>
+        <v>122</v>
+      </c>
+      <c r="T31" s="47">
+        <f>SUMIF(P$2:P$69,"&gt;=" &amp; R31,D$2:D$69)</f>
         <v>0</v>
       </c>
-      <c r="T31" s="47">
-        <f>SUMIF(P$2:P$68,"&gt;=" &amp; R31,D$2:D$68)</f>
-        <v>0</v>
-      </c>
       <c r="U31" s="9">
-        <f t="shared" si="0"/>
-        <v>3.9000000000000004</v>
+        <f t="shared" si="1"/>
+        <v>11.830000000000002</v>
       </c>
     </row>
     <row r="32" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="10"/>
       <c r="B32" s="23" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="C32" s="14">
         <v>4</v>
@@ -3346,7 +3297,7 @@
       <c r="N32" s="36"/>
       <c r="O32" s="34"/>
       <c r="P32" s="77">
-        <f>SUM(L32:O32)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q32" s="15"/>
@@ -3356,7 +3307,7 @@
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B33" s="23" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="C33" s="14">
         <v>5</v>
@@ -3383,23 +3334,25 @@
       <c r="M33" s="34">
         <v>0.5</v>
       </c>
-      <c r="N33" s="36"/>
+      <c r="N33" s="36">
+        <v>1</v>
+      </c>
       <c r="O33" s="34"/>
       <c r="P33" s="77">
-        <f>SUM(L33:O33)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4.5</v>
       </c>
       <c r="Q33" s="15"/>
     </row>
     <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B34" s="23" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C34" s="14">
         <v>2</v>
       </c>
       <c r="I34" s="22" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="J34" s="36">
         <v>0.5</v>
@@ -3408,17 +3361,19 @@
       <c r="M34" s="34">
         <v>0.5</v>
       </c>
-      <c r="N34" s="36"/>
+      <c r="N34" s="36">
+        <v>1</v>
+      </c>
       <c r="O34" s="34"/>
       <c r="P34" s="77">
-        <f>SUM(L34:O34)</f>
-        <v>0.5</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="Q34" s="15"/>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B35" s="23" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C35" s="14">
         <v>5</v>
@@ -3442,18 +3397,20 @@
       <c r="M35" s="34">
         <v>1</v>
       </c>
-      <c r="N35" s="36"/>
+      <c r="N35" s="36">
+        <v>1</v>
+      </c>
       <c r="O35" s="34"/>
       <c r="P35" s="77">
-        <f>SUM(L35:O35)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q35" s="15"/>
       <c r="R35" s="84"/>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B36" s="23" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="C36" s="14">
         <v>8</v>
@@ -3474,18 +3431,20 @@
       <c r="M36" s="34">
         <v>0.5</v>
       </c>
-      <c r="N36" s="36"/>
+      <c r="N36" s="36">
+        <v>1</v>
+      </c>
       <c r="O36" s="34"/>
       <c r="P36" s="77">
-        <f>SUM(L36:O36)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="Q36" s="15"/>
       <c r="R36" s="84"/>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B37" s="23" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C37" s="14">
         <v>4</v>
@@ -3506,10 +3465,13 @@
       <c r="M37" s="2">
         <v>0.8</v>
       </c>
+      <c r="N37" s="20">
+        <v>1</v>
+      </c>
       <c r="O37" s="34"/>
       <c r="P37" s="77">
-        <f>SUM(L37:O37)</f>
-        <v>0.8</v>
+        <f t="shared" si="0"/>
+        <v>2.8</v>
       </c>
       <c r="Q37" s="15"/>
       <c r="R37" s="84"/>
@@ -3517,10 +3479,10 @@
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="11" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C38" s="13">
         <v>6</v>
@@ -3549,18 +3511,20 @@
       <c r="M38" s="12">
         <v>1</v>
       </c>
-      <c r="N38" s="12"/>
+      <c r="N38" s="12">
+        <v>1</v>
+      </c>
       <c r="O38" s="35"/>
       <c r="P38" s="78">
-        <f>SUM(L38:O38)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q38" s="15"/>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="30"/>
       <c r="B39" s="31" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="C39" s="14">
         <v>6</v>
@@ -3584,11 +3548,13 @@
       <c r="M39" s="36">
         <v>0.75</v>
       </c>
-      <c r="N39" s="36"/>
+      <c r="N39" s="36">
+        <v>1</v>
+      </c>
       <c r="O39" s="36"/>
       <c r="P39" s="77">
-        <f>SUM(L39:O39)</f>
-        <v>1.75</v>
+        <f t="shared" si="0"/>
+        <v>3.75</v>
       </c>
       <c r="Q39" s="15"/>
       <c r="R39" s="15"/>
@@ -3597,7 +3563,7 @@
     <row r="40" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="30"/>
       <c r="B40" s="31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C40" s="14">
         <v>3</v>
@@ -3626,11 +3592,13 @@
       <c r="M40" s="36">
         <v>0.5</v>
       </c>
-      <c r="N40" s="36"/>
+      <c r="N40" s="36">
+        <v>1</v>
+      </c>
       <c r="O40" s="36"/>
       <c r="P40" s="77">
-        <f>SUM(L40:O40)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q40" s="15"/>
       <c r="R40" s="3"/>
@@ -3644,7 +3612,7 @@
     <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="30"/>
       <c r="B41" s="31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C41" s="14">
         <v>6</v>
@@ -3660,7 +3628,7 @@
       <c r="N41" s="36"/>
       <c r="O41" s="36"/>
       <c r="P41" s="77">
-        <f>SUM(L41:O41)</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="Q41" s="15"/>
@@ -3672,7 +3640,7 @@
     <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="30"/>
       <c r="B42" s="31" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="C42" s="14">
         <v>5</v>
@@ -3699,11 +3667,13 @@
       <c r="M42" s="36">
         <v>0</v>
       </c>
-      <c r="N42" s="36"/>
+      <c r="N42" s="36">
+        <v>1</v>
+      </c>
       <c r="O42" s="36"/>
       <c r="P42" s="77">
-        <f>SUM(L42:O42)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q42" s="15"/>
       <c r="U42" s="6"/>
@@ -3711,7 +3681,7 @@
     <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="30"/>
       <c r="B43" s="31" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="C43" s="14">
         <v>6</v>
@@ -3735,11 +3705,13 @@
       <c r="M43" s="36">
         <v>1</v>
       </c>
-      <c r="N43" s="36"/>
+      <c r="N43" s="36">
+        <v>1</v>
+      </c>
       <c r="O43" s="36"/>
       <c r="P43" s="77">
-        <f>SUM(L43:O43)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q43" s="15"/>
       <c r="R43" s="15"/>
@@ -3748,7 +3720,7 @@
     <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="30"/>
       <c r="B44" s="31" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="C44" s="14">
         <v>4</v>
@@ -3772,11 +3744,13 @@
       <c r="M44" s="36">
         <v>0.75</v>
       </c>
-      <c r="N44" s="36"/>
+      <c r="N44" s="36">
+        <v>1</v>
+      </c>
       <c r="O44" s="36"/>
       <c r="P44" s="77">
-        <f>SUM(L44:O44)</f>
-        <v>1.75</v>
+        <f t="shared" si="0"/>
+        <v>3.75</v>
       </c>
       <c r="Q44" s="15"/>
       <c r="T44" s="6"/>
@@ -3784,7 +3758,7 @@
     <row r="45" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="30"/>
       <c r="B45" s="31" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="C45" s="14">
         <v>7</v>
@@ -3813,11 +3787,13 @@
       <c r="M45" s="36">
         <v>1</v>
       </c>
-      <c r="N45" s="36"/>
+      <c r="N45" s="36">
+        <v>1</v>
+      </c>
       <c r="O45" s="36"/>
       <c r="P45" s="77">
-        <f>SUM(L45:O45)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q45" s="15"/>
       <c r="R45" s="3"/>
@@ -3832,7 +3808,7 @@
     <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="30"/>
       <c r="B46" s="31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C46" s="14">
         <v>6</v>
@@ -3857,17 +3833,19 @@
       <c r="M46" s="36">
         <v>0</v>
       </c>
-      <c r="N46" s="36"/>
+      <c r="N46" s="36">
+        <v>1</v>
+      </c>
       <c r="O46" s="36"/>
       <c r="P46" s="77">
-        <f>SUM(L46:O46)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="Q46" s="15"/>
     </row>
     <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B47" s="23" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C47" s="14">
         <v>5</v>
@@ -3894,19 +3872,22 @@
       <c r="M47" s="2">
         <v>1</v>
       </c>
+      <c r="N47" s="20">
+        <v>1</v>
+      </c>
       <c r="O47" s="34"/>
       <c r="P47" s="77">
-        <f>SUM(L47:O47)</f>
-        <v>1.5</v>
+        <f t="shared" si="0"/>
+        <v>4</v>
       </c>
       <c r="Q47" s="15"/>
     </row>
     <row r="48" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C48" s="13">
         <v>2</v>
@@ -3933,11 +3914,13 @@
       <c r="M48" s="12">
         <v>0</v>
       </c>
-      <c r="N48" s="12"/>
+      <c r="N48" s="12">
+        <v>1</v>
+      </c>
       <c r="O48" s="35"/>
       <c r="P48" s="78">
-        <f>SUM(L48:O48)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2.5</v>
       </c>
       <c r="Q48" s="15"/>
       <c r="R48" s="15"/>
@@ -3949,7 +3932,7 @@
     </row>
     <row r="49" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B49" s="23" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C49" s="14">
         <v>7</v>
@@ -3976,10 +3959,13 @@
       <c r="M49" s="2">
         <v>0.7</v>
       </c>
+      <c r="N49" s="20">
+        <v>1</v>
+      </c>
       <c r="O49" s="34"/>
       <c r="P49" s="77">
-        <f>SUM(L49:O49)</f>
-        <v>1.7</v>
+        <f t="shared" si="0"/>
+        <v>4.7</v>
       </c>
       <c r="Q49" s="15"/>
       <c r="V49" s="33"/>
@@ -3990,7 +3976,7 @@
     <row r="50" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="10"/>
       <c r="B50" s="23" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C50" s="14">
         <v>4</v>
@@ -4019,11 +4005,13 @@
       <c r="M50" s="2">
         <v>1</v>
       </c>
-      <c r="N50" s="20"/>
+      <c r="N50" s="20">
+        <v>1</v>
+      </c>
       <c r="O50" s="34"/>
       <c r="P50" s="77">
-        <f>SUM(L50:O50)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q50" s="15"/>
       <c r="R50" s="3"/>
@@ -4037,7 +4025,7 @@
     </row>
     <row r="51" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B51" s="23" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C51" s="14">
         <v>3</v>
@@ -4051,15 +4039,15 @@
       </c>
       <c r="O51" s="34"/>
       <c r="P51" s="77">
-        <f>SUM(L51:O51)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>0.5</v>
       </c>
       <c r="Q51" s="15"/>
       <c r="V51" s="33"/>
     </row>
     <row r="52" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B52" s="23" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C52" s="14">
         <v>4</v>
@@ -4070,7 +4058,7 @@
       </c>
       <c r="O52" s="34"/>
       <c r="P52" s="77">
-        <f>SUM(L52:O52)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q52" s="15"/>
@@ -4078,7 +4066,7 @@
     </row>
     <row r="53" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B53" s="23" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C53" s="14">
         <v>6</v>
@@ -4095,7 +4083,7 @@
       </c>
       <c r="O53" s="34"/>
       <c r="P53" s="77">
-        <f>SUM(L53:O53)</f>
+        <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
       <c r="Q53" s="15"/>
@@ -4104,7 +4092,7 @@
     </row>
     <row r="54" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B54" s="23" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="C54" s="14">
         <v>3</v>
@@ -4131,20 +4119,23 @@
       <c r="M54" s="2">
         <v>1</v>
       </c>
+      <c r="N54" s="20">
+        <v>1</v>
+      </c>
       <c r="O54" s="34"/>
       <c r="P54" s="77">
-        <f>SUM(L54:O54)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q54" s="15"/>
       <c r="V54" s="33"/>
     </row>
     <row r="55" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A55" s="11" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="C55" s="13">
         <v>2</v>
@@ -4169,11 +4160,13 @@
       <c r="M55" s="12">
         <v>1</v>
       </c>
-      <c r="N55" s="12"/>
+      <c r="N55" s="12">
+        <v>1</v>
+      </c>
       <c r="O55" s="35"/>
       <c r="P55" s="78">
-        <f>SUM(L55:O55)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>3</v>
       </c>
       <c r="Q55" s="15"/>
       <c r="U55" s="6"/>
@@ -4181,7 +4174,7 @@
     </row>
     <row r="56" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B56" s="23" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C56" s="14">
         <v>7</v>
@@ -4208,17 +4201,20 @@
       <c r="M56" s="2">
         <v>1</v>
       </c>
+      <c r="N56" s="20">
+        <v>1</v>
+      </c>
       <c r="O56" s="34"/>
       <c r="P56" s="77">
-        <f>SUM(L56:O56)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q56" s="15"/>
       <c r="V56" s="33"/>
     </row>
     <row r="57" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B57" s="23" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="C57" s="14">
         <v>2</v>
@@ -4245,10 +4241,13 @@
       <c r="M57" s="2">
         <v>1</v>
       </c>
+      <c r="N57" s="20">
+        <v>1</v>
+      </c>
       <c r="O57" s="34"/>
       <c r="P57" s="77">
-        <f>SUM(L57:O57)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>5</v>
       </c>
       <c r="Q57" s="15"/>
       <c r="V57" s="33"/>
@@ -4258,7 +4257,7 @@
     </row>
     <row r="58" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B58" s="23" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
       <c r="C58" s="14">
         <v>3</v>
@@ -4269,7 +4268,7 @@
       </c>
       <c r="O58" s="34"/>
       <c r="P58" s="77">
-        <f>SUM(L58:O58)</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="Q58" s="15"/>
@@ -4277,10 +4276,10 @@
     </row>
     <row r="59" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A59" s="11" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C59" s="13">
         <v>4</v>
@@ -4304,8 +4303,8 @@
       <c r="N59" s="12"/>
       <c r="O59" s="35"/>
       <c r="P59" s="78">
-        <f>SUM(L59:O59)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="Q59" s="15"/>
       <c r="U59" s="6"/>
@@ -4313,7 +4312,7 @@
     </row>
     <row r="60" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B60" s="23" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C60" s="14">
         <v>3</v>
@@ -4330,8 +4329,8 @@
       </c>
       <c r="O60" s="34"/>
       <c r="P60" s="77">
-        <f>SUM(L60:O60)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
       <c r="Q60" s="15"/>
       <c r="V60" s="33"/>
@@ -4365,7 +4364,7 @@
       <c r="N61" s="12"/>
       <c r="O61" s="35"/>
       <c r="P61" s="78">
-        <f>SUM(L61:O61)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q61" s="15"/>
@@ -4386,10 +4385,12 @@
       <c r="M62" s="20">
         <v>1</v>
       </c>
-      <c r="O62" s="36"/>
+      <c r="O62" s="36">
+        <v>1</v>
+      </c>
       <c r="P62" s="77">
-        <f>SUM(L62:O62)</f>
-        <v>1</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="Q62" s="15"/>
     </row>
@@ -4418,10 +4419,12 @@
         <v>1</v>
       </c>
       <c r="N63" s="20"/>
-      <c r="O63" s="34"/>
+      <c r="O63" s="34">
+        <v>-2</v>
+      </c>
       <c r="P63" s="77">
-        <f>SUM(L63:O63)</f>
-        <v>2</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="Q63" s="15"/>
       <c r="R63" s="3"/>
@@ -4452,298 +4455,322 @@
       </c>
       <c r="O64" s="34"/>
       <c r="P64" s="77">
-        <f>SUM(L64:O64)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q64" s="15"/>
       <c r="S64" s="33"/>
       <c r="U64" s="6"/>
     </row>
-    <row r="65" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="10"/>
       <c r="B65" s="23" t="s">
-        <v>95</v>
+        <v>181</v>
       </c>
       <c r="C65" s="14">
         <v>1</v>
       </c>
-      <c r="D65" s="14">
-        <v>0</v>
-      </c>
-      <c r="I65" s="22" t="s">
-        <v>91</v>
-      </c>
-      <c r="K65" s="36">
-        <v>1</v>
-      </c>
-      <c r="M65" s="2">
-        <v>0</v>
-      </c>
-      <c r="O65" s="34"/>
+      <c r="D65" s="14"/>
+      <c r="E65" s="14"/>
+      <c r="F65" s="14"/>
+      <c r="G65" s="14"/>
+      <c r="H65" s="14"/>
+      <c r="I65" s="22"/>
+      <c r="J65" s="36"/>
+      <c r="K65" s="36"/>
+      <c r="L65" s="34"/>
+      <c r="M65" s="34"/>
+      <c r="N65" s="36"/>
+      <c r="O65" s="34">
+        <v>2</v>
+      </c>
       <c r="P65" s="77">
-        <f>SUM(L65:O65)</f>
-        <v>0</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
       <c r="Q65" s="15"/>
-      <c r="V65" s="6"/>
-      <c r="W65" s="6"/>
-      <c r="X65" s="6"/>
-      <c r="Y65" s="6"/>
+      <c r="R65" s="3"/>
+      <c r="U65" s="6"/>
     </row>
     <row r="66" spans="1:25" x14ac:dyDescent="0.3">
       <c r="B66" s="23" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C66" s="14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D66" s="14">
-        <v>1</v>
-      </c>
-      <c r="I66" s="22"/>
-      <c r="L66" s="2">
+        <v>0</v>
+      </c>
+      <c r="I66" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="K66" s="36">
         <v>1</v>
       </c>
       <c r="M66" s="2">
+        <v>0</v>
+      </c>
+      <c r="N66" s="20">
         <v>1</v>
       </c>
       <c r="O66" s="34"/>
       <c r="P66" s="77">
-        <f>SUM(L66:O66)</f>
+        <f t="shared" si="0"/>
         <v>2</v>
       </c>
       <c r="Q66" s="15"/>
-    </row>
-    <row r="67" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="10"/>
-      <c r="B67" s="24" t="s">
+      <c r="V66" s="6"/>
+      <c r="W66" s="6"/>
+      <c r="X66" s="6"/>
+      <c r="Y66" s="6"/>
+    </row>
+    <row r="67" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B67" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C67" s="14">
+        <v>3</v>
+      </c>
+      <c r="D67" s="14">
+        <v>1</v>
+      </c>
+      <c r="I67" s="22"/>
+      <c r="L67" s="2">
+        <v>1</v>
+      </c>
+      <c r="M67" s="2">
+        <v>1</v>
+      </c>
+      <c r="O67" s="34"/>
+      <c r="P67" s="77">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Q67" s="15"/>
+    </row>
+    <row r="68" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="10"/>
+      <c r="B68" s="24" t="s">
         <v>97</v>
       </c>
-      <c r="C67" s="27">
+      <c r="C68" s="27">
         <v>4</v>
       </c>
-      <c r="D67" s="27">
+      <c r="D68" s="27">
         <v>0</v>
       </c>
-      <c r="E67" s="27"/>
-      <c r="F67" s="27"/>
-      <c r="G67" s="27"/>
-      <c r="H67" s="27"/>
-      <c r="I67" s="29"/>
-      <c r="J67" s="37"/>
-      <c r="K67" s="37"/>
-      <c r="L67" s="28">
-        <v>1</v>
-      </c>
-      <c r="M67" s="28">
+      <c r="E68" s="27"/>
+      <c r="F68" s="27"/>
+      <c r="G68" s="27"/>
+      <c r="H68" s="27"/>
+      <c r="I68" s="29"/>
+      <c r="J68" s="37"/>
+      <c r="K68" s="37"/>
+      <c r="L68" s="28">
+        <v>1</v>
+      </c>
+      <c r="M68" s="28">
         <v>0</v>
       </c>
-      <c r="N67" s="28"/>
-      <c r="O67" s="37"/>
-      <c r="P67" s="79">
-        <f>SUM(L67:O67)</f>
-        <v>1</v>
-      </c>
-      <c r="Q67" s="15"/>
-      <c r="R67" s="3"/>
-      <c r="S67"/>
-      <c r="T67"/>
-      <c r="U67"/>
-      <c r="V67"/>
-      <c r="W67"/>
-      <c r="X67"/>
-      <c r="Y67"/>
-    </row>
-    <row r="68" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="11"/>
+      <c r="N68" s="28"/>
+      <c r="O68" s="37"/>
+      <c r="P68" s="79">
+        <f t="shared" ref="P68" si="2">SUM(J68:O68)</f>
+        <v>1</v>
+      </c>
       <c r="Q68" s="15"/>
-    </row>
-    <row r="69" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I69" s="64" t="s">
+      <c r="R68" s="3"/>
+      <c r="S68"/>
+      <c r="T68"/>
+      <c r="U68"/>
+      <c r="V68"/>
+      <c r="W68"/>
+      <c r="X68"/>
+      <c r="Y68"/>
+    </row>
+    <row r="69" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="11"/>
+      <c r="Q69" s="15"/>
+    </row>
+    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I70" s="64" t="s">
         <v>98</v>
       </c>
-      <c r="J69" s="85"/>
-      <c r="K69" s="85"/>
-      <c r="L69" s="65">
-        <f t="array" ref="L69">SUM($C2:$C67*(L2:L67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>178</v>
-      </c>
-      <c r="M69" s="65">
-        <f t="array" ref="M69">SUM($C2:$C67*(M2:M67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>110</v>
-      </c>
-      <c r="N69" s="65">
-        <f t="array" ref="N69">SUM($C2:$C67*(N2:N67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="O69" s="66">
-        <f t="array" ref="O69">SUM($C2:$C67*(O2:O67&gt;=0.9)*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="Q69" s="15"/>
-      <c r="T69" s="33"/>
-    </row>
-    <row r="70" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="I70" s="67" t="s">
-        <v>100</v>
-      </c>
-      <c r="J70" s="86"/>
-      <c r="K70" s="86"/>
-      <c r="L70" s="68">
-        <f t="array" ref="L70">SUM($C2:$C67*L2:L67*($P2:$P67&gt;=$R$12))</f>
-        <v>180.5</v>
-      </c>
-      <c r="M70" s="68">
-        <f t="array" ref="M70">SUM($C2:$C67*M2:M67*($P2:$P67&gt;=$R$12))</f>
-        <v>154.80000000000001</v>
-      </c>
-      <c r="N70" s="68">
-        <f t="array" ref="N70">SUM($C2:$C67*N2:N67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="O70" s="69">
-        <f t="array" ref="O70">SUM($C2:$C67*O2:O67*($P2:$P67&gt;=$R$12))</f>
-        <v>0</v>
+      <c r="J70" s="85"/>
+      <c r="K70" s="85"/>
+      <c r="L70" s="65">
+        <f t="array" ref="L70">SUM($C2:$C68*(L2:L68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
+        <v>184</v>
+      </c>
+      <c r="M70" s="65">
+        <f t="array" ref="M70">SUM($C2:$C68*(M2:M68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
+        <v>111</v>
+      </c>
+      <c r="N70" s="65">
+        <f t="array" ref="N70">SUM($C2:$C68*(N2:N68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
+        <v>200</v>
+      </c>
+      <c r="O70" s="66">
+        <f t="array" ref="O70">SUM($C2:$C68*(O2:O68&gt;=0.9)*($P2:$P68&gt;=$R$12))</f>
+        <v>8</v>
       </c>
       <c r="Q70" s="15"/>
-      <c r="V70" s="6"/>
-      <c r="W70" s="6"/>
-      <c r="X70" s="6"/>
-      <c r="Y70" s="6"/>
+      <c r="T70" s="33"/>
     </row>
     <row r="71" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I71" s="67" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="J71" s="86"/>
       <c r="K71" s="86"/>
       <c r="L71" s="68">
-        <f t="array" ref="L71">SUM($C$2:$C$67*(L$2:L$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>183</v>
+        <f t="array" ref="L71">SUM($C2:$C68*L2:L68*($P2:$P68&gt;=$R$12))</f>
+        <v>189</v>
       </c>
       <c r="M71" s="68">
-        <f t="array" ref="M71">SUM($C$2:$C$67*(M$2:M$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>183</v>
+        <f t="array" ref="M71">SUM($C2:$C68*M2:M68*($P2:$P68&gt;=$R$12))</f>
+        <v>168.25000000000003</v>
       </c>
       <c r="N71" s="68">
-        <f t="array" ref="N71">SUM($C$2:$C$67*(N$2:N$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>0</v>
+        <f t="array" ref="N71">SUM($C2:$C68*N2:N68*($P2:$P68&gt;=$R$12))</f>
+        <v>200</v>
       </c>
       <c r="O71" s="69">
-        <f t="array" ref="O71">SUM($C$2:$C$67*(O$2:O$67&gt;=0.1)*($P$2:$P$67&gt;=$R$12))</f>
-        <v>0</v>
+        <f t="array" ref="O71">SUM($C2:$C68*O2:O68*($P2:$P68&gt;=$R$12))</f>
+        <v>9</v>
       </c>
       <c r="Q71" s="15"/>
-    </row>
-    <row r="72" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="10"/>
-      <c r="B72" s="23"/>
-      <c r="C72" s="14"/>
-      <c r="D72" s="14"/>
-      <c r="E72" s="14"/>
-      <c r="F72" s="14"/>
-      <c r="G72" s="14"/>
-      <c r="H72" s="14"/>
+      <c r="V71" s="6"/>
+      <c r="W71" s="6"/>
+      <c r="X71" s="6"/>
+      <c r="Y71" s="6"/>
+    </row>
+    <row r="72" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I72" s="67" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="J72" s="86"/>
       <c r="K72" s="86"/>
       <c r="L72" s="68">
-        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>183</v>
+        <f t="array" ref="L72">SUM($C$2:$C$68*(L$2:L$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>194</v>
       </c>
       <c r="M72" s="68">
-        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>183</v>
+        <f t="array" ref="M72">SUM($C$2:$C$68*(M$2:M$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>204</v>
       </c>
       <c r="N72" s="68">
-        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>183</v>
+        <f t="array" ref="N72">SUM($C$2:$C$68*(N$2:N$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>200</v>
       </c>
       <c r="O72" s="69">
-        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
-        <v>183</v>
-      </c>
-      <c r="P72" s="3"/>
+        <f t="array" ref="O72">SUM($C$2:$C$68*(O$2:O$68&gt;=0.1)*($P$2:$P$68&gt;=$R$12))</f>
+        <v>8</v>
+      </c>
       <c r="Q72" s="15"/>
-      <c r="R72" s="3"/>
-      <c r="S72"/>
-      <c r="T72"/>
-      <c r="U72"/>
-      <c r="V72"/>
-      <c r="W72"/>
-      <c r="X72"/>
-      <c r="Y72"/>
-    </row>
-    <row r="73" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="73" spans="1:25" s="6" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="10"/>
+      <c r="B73" s="23"/>
+      <c r="C73" s="14"/>
+      <c r="D73" s="14"/>
+      <c r="E73" s="14"/>
+      <c r="F73" s="14"/>
+      <c r="G73" s="14"/>
+      <c r="H73" s="14"/>
       <c r="I73" s="67" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="J73" s="86"/>
       <c r="K73" s="86"/>
-      <c r="L73" s="70">
-        <f t="shared" ref="L73:O73" si="1">L70/L72</f>
-        <v>0.98633879781420764</v>
-      </c>
-      <c r="M73" s="70">
-        <f t="shared" si="1"/>
-        <v>0.84590163934426232</v>
-      </c>
-      <c r="N73" s="70">
-        <f t="shared" si="1"/>
+      <c r="L73" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+        <v>223</v>
+      </c>
+      <c r="M73" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+        <v>223</v>
+      </c>
+      <c r="N73" s="68">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+        <v>223</v>
+      </c>
+      <c r="O73" s="69">
+        <f>LOOKUP($R$12,$R23:$R31,$S23:$S31)</f>
+        <v>223</v>
+      </c>
+      <c r="P73" s="3"/>
+      <c r="Q73" s="15"/>
+      <c r="R73" s="3"/>
+      <c r="S73"/>
+      <c r="T73"/>
+      <c r="U73"/>
+      <c r="V73"/>
+      <c r="W73"/>
+      <c r="X73"/>
+      <c r="Y73"/>
+    </row>
+    <row r="74" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I74" s="67" t="s">
+        <v>102</v>
+      </c>
+      <c r="J74" s="86"/>
+      <c r="K74" s="86"/>
+      <c r="L74" s="70">
+        <f t="shared" ref="L74:O74" si="3">L71/L73</f>
+        <v>0.84753363228699552</v>
+      </c>
+      <c r="M74" s="70">
+        <f t="shared" si="3"/>
+        <v>0.75448430493273555</v>
+      </c>
+      <c r="N74" s="70">
+        <f t="shared" si="3"/>
+        <v>0.89686098654708524</v>
+      </c>
+      <c r="O74" s="71">
+        <f t="shared" si="3"/>
+        <v>4.0358744394618833E-2</v>
+      </c>
+      <c r="Q74" s="15"/>
+      <c r="V74" s="6"/>
+      <c r="W74" s="6"/>
+      <c r="X74" s="6"/>
+      <c r="Y74" s="6"/>
+    </row>
+    <row r="75" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C75" s="33"/>
+      <c r="I75" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="J75" s="87"/>
+      <c r="K75" s="87"/>
+      <c r="L75" s="73">
+        <f t="array" ref="L75">SUM($C2:$C68*L2:L68*($P2:$P68&lt;$R$12))</f>
+        <v>6</v>
+      </c>
+      <c r="M75" s="73">
+        <f t="array" ref="M75">SUM($C2:$C68*M2:M68*($P2:$P68&lt;$R$12))</f>
+        <v>21.849999999999998</v>
+      </c>
+      <c r="N75" s="73">
+        <f t="array" ref="N75">SUM($C2:$C68*N2:N68*($P2:$P68&lt;$R$12))</f>
         <v>0</v>
       </c>
-      <c r="O73" s="71">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="Q73" s="15"/>
-      <c r="V73" s="6"/>
-      <c r="W73" s="6"/>
-      <c r="X73" s="6"/>
-      <c r="Y73" s="6"/>
-    </row>
-    <row r="74" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C74" s="33"/>
-      <c r="I74" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="J74" s="87"/>
-      <c r="K74" s="87"/>
-      <c r="L74" s="73">
-        <f t="array" ref="L74">SUM($C2:$C67*L2:L67*($P2:$P67&lt;$R$12))</f>
-        <v>15.5</v>
-      </c>
-      <c r="M74" s="73">
-        <f t="array" ref="M74">SUM($C2:$C67*M2:M67*($P2:$P67&lt;$R$12))</f>
-        <v>36.299999999999997</v>
-      </c>
-      <c r="N74" s="73">
-        <f t="array" ref="N74">SUM($C2:$C67*N2:N67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="O74" s="74">
-        <f t="array" ref="O74">SUM($C2:$C67*O2:O67*($P2:$P67&lt;$R$12))</f>
-        <v>0</v>
-      </c>
-      <c r="Q74" s="15"/>
-    </row>
-    <row r="75" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="C75" s="33"/>
+      <c r="O75" s="74">
+        <f t="array" ref="O75">SUM($C2:$C68*O2:O68*($P2:$P68&lt;$R$12))</f>
+        <v>-4</v>
+      </c>
       <c r="Q75" s="15"/>
-      <c r="V75" s="6"/>
-      <c r="W75" s="6"/>
-      <c r="X75" s="6"/>
-      <c r="Y75" s="6"/>
     </row>
     <row r="76" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C76" s="33"/>
-      <c r="I76" s="14"/>
-      <c r="J76" s="14"/>
-      <c r="K76" s="14"/>
-      <c r="L76" s="14"/>
-      <c r="M76" s="14"/>
       <c r="Q76" s="15"/>
+      <c r="V76" s="6"/>
+      <c r="W76" s="6"/>
+      <c r="X76" s="6"/>
+      <c r="Y76" s="6"/>
     </row>
     <row r="77" spans="1:25" x14ac:dyDescent="0.3">
       <c r="C77" s="33"/>
@@ -4755,6 +4782,7 @@
       <c r="Q77" s="15"/>
     </row>
     <row r="78" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="C78" s="33"/>
       <c r="I78" s="14"/>
       <c r="J78" s="14"/>
       <c r="K78" s="14"/>
@@ -4777,7 +4805,6 @@
       <c r="L80" s="14"/>
       <c r="M80" s="14"/>
       <c r="Q80" s="15"/>
-      <c r="U80" s="33"/>
     </row>
     <row r="81" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I81" s="14"/>
@@ -4786,6 +4813,7 @@
       <c r="L81" s="14"/>
       <c r="M81" s="14"/>
       <c r="Q81" s="15"/>
+      <c r="U81" s="33"/>
     </row>
     <row r="82" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I82" s="14"/>
@@ -4793,6 +4821,7 @@
       <c r="K82" s="14"/>
       <c r="L82" s="14"/>
       <c r="M82" s="14"/>
+      <c r="Q82" s="15"/>
     </row>
     <row r="83" spans="1:25" x14ac:dyDescent="0.3">
       <c r="I83" s="14"/>
@@ -4801,66 +4830,73 @@
       <c r="L83" s="14"/>
       <c r="M83" s="14"/>
     </row>
-    <row r="85" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A85" s="10"/>
-      <c r="B85" s="23"/>
-      <c r="C85" s="14"/>
-      <c r="D85" s="14"/>
-      <c r="E85" s="14"/>
-      <c r="F85" s="14"/>
-      <c r="G85" s="14"/>
-      <c r="H85" s="14"/>
-      <c r="I85" s="20"/>
-      <c r="J85" s="36"/>
-      <c r="K85" s="36"/>
-      <c r="L85" s="2"/>
-      <c r="M85" s="2"/>
-      <c r="N85" s="20"/>
-      <c r="O85" s="2"/>
-      <c r="P85" s="3"/>
-      <c r="Q85" s="3"/>
-      <c r="R85" s="3"/>
-      <c r="S85"/>
-      <c r="T85"/>
-      <c r="U85"/>
-      <c r="V85"/>
-      <c r="W85"/>
-      <c r="X85"/>
-      <c r="Y85"/>
-    </row>
-    <row r="88" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V88" s="6"/>
-      <c r="W88" s="6"/>
-      <c r="X88" s="6"/>
-      <c r="Y88" s="6"/>
-    </row>
-    <row r="92" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="V92" s="6"/>
-      <c r="W92" s="6"/>
-      <c r="X92" s="6"/>
-      <c r="Y92" s="6"/>
-    </row>
-    <row r="97" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V97" s="6"/>
-      <c r="W97" s="6"/>
-      <c r="X97" s="6"/>
-      <c r="Y97" s="6"/>
-    </row>
-    <row r="110" spans="22:25" x14ac:dyDescent="0.3">
-      <c r="V110" s="33"/>
-      <c r="W110" s="33"/>
-      <c r="X110" s="33"/>
-      <c r="Y110" s="33"/>
+    <row r="84" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="I84" s="14"/>
+      <c r="J84" s="14"/>
+      <c r="K84" s="14"/>
+      <c r="L84" s="14"/>
+      <c r="M84" s="14"/>
+    </row>
+    <row r="86" spans="1:25" s="33" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="10"/>
+      <c r="B86" s="23"/>
+      <c r="C86" s="14"/>
+      <c r="D86" s="14"/>
+      <c r="E86" s="14"/>
+      <c r="F86" s="14"/>
+      <c r="G86" s="14"/>
+      <c r="H86" s="14"/>
+      <c r="I86" s="20"/>
+      <c r="J86" s="36"/>
+      <c r="K86" s="36"/>
+      <c r="L86" s="2"/>
+      <c r="M86" s="2"/>
+      <c r="N86" s="20"/>
+      <c r="O86" s="2"/>
+      <c r="P86" s="3"/>
+      <c r="Q86" s="3"/>
+      <c r="R86" s="3"/>
+      <c r="S86"/>
+      <c r="T86"/>
+      <c r="U86"/>
+      <c r="V86"/>
+      <c r="W86"/>
+      <c r="X86"/>
+      <c r="Y86"/>
+    </row>
+    <row r="89" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V89" s="6"/>
+      <c r="W89" s="6"/>
+      <c r="X89" s="6"/>
+      <c r="Y89" s="6"/>
+    </row>
+    <row r="93" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="V93" s="6"/>
+      <c r="W93" s="6"/>
+      <c r="X93" s="6"/>
+      <c r="Y93" s="6"/>
+    </row>
+    <row r="98" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V98" s="6"/>
+      <c r="W98" s="6"/>
+      <c r="X98" s="6"/>
+      <c r="Y98" s="6"/>
+    </row>
+    <row r="111" spans="22:25" x14ac:dyDescent="0.3">
+      <c r="V111" s="33"/>
+      <c r="W111" s="33"/>
+      <c r="X111" s="33"/>
+      <c r="Y111" s="33"/>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="B2:P67">
-    <cfRule type="expression" dxfId="14" priority="31" stopIfTrue="1">
+  <conditionalFormatting sqref="B2:P68">
+    <cfRule type="expression" dxfId="2" priority="31" stopIfTrue="1">
       <formula>$P2&gt;=(0.5+$R$12)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="32" stopIfTrue="1">
       <formula>$P2&gt;=$R$12</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="33">
+    <cfRule type="expression" dxfId="0" priority="33">
       <formula>$P2&gt;=($R$12-0.5)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>